<commit_message>
Checkpoint before major changes
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Keys" sheetId="2" r:id="rId1"/>
+    <sheet name="Layers" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="142">
-  <si>
-    <t>Key Down</t>
-  </si>
-  <si>
-    <t>Key Up</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
   <si>
     <t>a</t>
   </si>
@@ -440,17 +435,44 @@
     <t>Layer</t>
   </si>
   <si>
-    <t>Layer Keys</t>
-  </si>
-  <si>
-    <t>edit</t>
-  </si>
-  <si>
-    <t>select</t>
-  </si>
-  <si>
-    <t>f
-d</t>
+    <t>Alpha Down</t>
+  </si>
+  <si>
+    <t>Alpha Up</t>
+  </si>
+  <si>
+    <t>Edit Down</t>
+  </si>
+  <si>
+    <t>Edit Up</t>
+  </si>
+  <si>
+    <t>{Shift Down}</t>
+  </si>
+  <si>
+    <t>{Shift Up}</t>
+  </si>
+  <si>
+    <t>{Up}</t>
+  </si>
+  <si>
+    <t>{Left}</t>
+  </si>
+  <si>
+    <t>{Down}</t>
+  </si>
+  <si>
+    <t>{Right}</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>d
+f</t>
   </si>
 </sst>
 </file>
@@ -508,7 +530,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -526,12 +552,23 @@
   <autoFilter ref="A1:G58"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Hotkey"/>
-    <tableColumn id="2" name="Key Down"/>
-    <tableColumn id="3" name="Key Up"/>
+    <tableColumn id="2" name="Alpha Down"/>
+    <tableColumn id="3" name="Alpha Up"/>
     <tableColumn id="4" name="Green Down"/>
     <tableColumn id="5" name="Green Up"/>
-    <tableColumn id="6" name="Layer"/>
-    <tableColumn id="7" name="Layer Keys"/>
+    <tableColumn id="6" name="Edit Down"/>
+    <tableColumn id="7" name="Edit Up"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Layer"/>
+    <tableColumn id="2" name="Keys" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -802,287 +839,288 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
         <v>96</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" t="s">
-        <v>139</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="F12" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="F13" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="F15" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F22" t="s">
         <v>140</v>
@@ -1093,290 +1131,290 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" t="s">
         <v>132</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D29" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1388,4 +1426,38 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Basic functionality of TextBlade with Excel for hotkeys.
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Keys" sheetId="2" r:id="rId1"/>
-    <sheet name="Layers" sheetId="3" r:id="rId2"/>
+    <sheet name="Keys" sheetId="4" r:id="rId1"/>
+    <sheet name="Keys.Orig" sheetId="2" r:id="rId2"/>
+    <sheet name="Layers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="211">
   <si>
     <t>a</t>
   </si>
@@ -473,6 +474,201 @@
   <si>
     <t>d
 f</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>a
+s
+d
+f</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>FunctionLow</t>
+  </si>
+  <si>
+    <t>FunctionHigh</t>
+  </si>
+  <si>
+    <t>l
+;</t>
+  </si>
+  <si>
+    <t>^x</t>
+  </si>
+  <si>
+    <t>^c</t>
+  </si>
+  <si>
+    <t>^v</t>
+  </si>
+  <si>
+    <t>^z</t>
+  </si>
+  <si>
+    <t>^y</t>
+  </si>
+  <si>
+    <t>^{Home}</t>
+  </si>
+  <si>
+    <t>{Home}</t>
+  </si>
+  <si>
+    <t>{End}</t>
+  </si>
+  <si>
+    <t>^{End}</t>
+  </si>
+  <si>
+    <t>FunctionLow Down</t>
+  </si>
+  <si>
+    <t>FunctionLow Up</t>
+  </si>
+  <si>
+    <t>{F1}</t>
+  </si>
+  <si>
+    <t>{F2}</t>
+  </si>
+  <si>
+    <t>{F3}</t>
+  </si>
+  <si>
+    <t>{F4}</t>
+  </si>
+  <si>
+    <t>{F5}</t>
+  </si>
+  <si>
+    <t>{F10}</t>
+  </si>
+  <si>
+    <t>{F11}</t>
+  </si>
+  <si>
+    <t>{F12}</t>
+  </si>
+  <si>
+    <t>{F13}</t>
+  </si>
+  <si>
+    <t>{F14}</t>
+  </si>
+  <si>
+    <t>{F15}</t>
+  </si>
+  <si>
+    <t>{F6}</t>
+  </si>
+  <si>
+    <t>{F7}</t>
+  </si>
+  <si>
+    <t>{F8}</t>
+  </si>
+  <si>
+    <t>{F9}</t>
+  </si>
+  <si>
+    <t>{F16}</t>
+  </si>
+  <si>
+    <t>{F17}</t>
+  </si>
+  <si>
+    <t>{F18}</t>
+  </si>
+  <si>
+    <t>{F19}</t>
+  </si>
+  <si>
+    <t>{F20}</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>+2</t>
+  </si>
+  <si>
+    <t>+3</t>
+  </si>
+  <si>
+    <t>+4</t>
+  </si>
+  <si>
+    <t>+5</t>
+  </si>
+  <si>
+    <t>+6</t>
+  </si>
+  <si>
+    <t>+7</t>
+  </si>
+  <si>
+    <t>+8</t>
+  </si>
+  <si>
+    <t>+9</t>
+  </si>
+  <si>
+    <t>+0</t>
+  </si>
+  <si>
+    <t>+=</t>
+  </si>
+  <si>
+    <t>+-</t>
+  </si>
+  <si>
+    <t>+`</t>
+  </si>
+  <si>
+    <t>{Escape}</t>
+  </si>
+  <si>
+    <t>{Volume_Up}</t>
+  </si>
+  <si>
+    <t>Media Down</t>
+  </si>
+  <si>
+    <t>Media Up</t>
+  </si>
+  <si>
+    <t>{Volume_Down}</t>
+  </si>
+  <si>
+    <t>{Volume_Mute}</t>
+  </si>
+  <si>
+    <t>k
+l</t>
+  </si>
+  <si>
+    <t>Green Media</t>
+  </si>
+  <si>
+    <t>Space
+a
+s
+d
+f</t>
+  </si>
+  <si>
+    <t>Green Media Up</t>
+  </si>
+  <si>
+    <t>Green Media Down</t>
   </si>
 </sst>
 </file>
@@ -548,9 +744,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys" displayName="HotKeys" ref="A1:G58" totalsRowShown="0">
-  <autoFilter ref="A1:G58"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys" displayName="HotKeys" ref="A1:M71" totalsRowShown="0">
+  <autoFilter ref="A1:M71"/>
+  <tableColumns count="13">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
     <tableColumn id="3" name="Alpha Up"/>
@@ -558,17 +754,42 @@
     <tableColumn id="5" name="Green Up"/>
     <tableColumn id="6" name="Edit Down"/>
     <tableColumn id="7" name="Edit Up"/>
+    <tableColumn id="8" name="FunctionLow Down"/>
+    <tableColumn id="9" name="FunctionLow Up"/>
+    <tableColumn id="11" name="Media Down"/>
+    <tableColumn id="12" name="Media Up"/>
+    <tableColumn id="10" name="Green Media Down"/>
+    <tableColumn id="13" name="Green Media Up"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys_orig" displayName="HotKeys_orig" ref="A1:I58" totalsRowShown="0">
+  <autoFilter ref="A1:I58"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Hotkey"/>
+    <tableColumn id="2" name="Alpha Down"/>
+    <tableColumn id="3" name="Alpha Up"/>
+    <tableColumn id="4" name="Green Down"/>
+    <tableColumn id="5" name="Green Up"/>
+    <tableColumn id="6" name="Edit Down"/>
+    <tableColumn id="7" name="Edit Up"/>
+    <tableColumn id="8" name="FunctionLow Down"/>
+    <tableColumn id="9" name="FunctionLow Up"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="Layer"/>
     <tableColumn id="2" name="Keys" dataDxfId="0"/>
+    <tableColumn id="3" name="Delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,13 +1058,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,9 +1076,15 @@
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -879,8 +1106,893 @@
       <c r="G1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" t="s">
+        <v>210</v>
+      </c>
+      <c r="M1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
+        <v>156</v>
+      </c>
+      <c r="H22" t="s">
+        <v>178</v>
+      </c>
+      <c r="I22" t="s">
+        <v>182</v>
+      </c>
+      <c r="L22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H23" t="s">
+        <v>179</v>
+      </c>
+      <c r="I23" t="s">
+        <v>183</v>
+      </c>
+      <c r="L23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" t="s">
+        <v>142</v>
+      </c>
+      <c r="H24" t="s">
+        <v>180</v>
+      </c>
+      <c r="I24" t="s">
+        <v>184</v>
+      </c>
+      <c r="J24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" t="s">
+        <v>181</v>
+      </c>
+      <c r="I25" t="s">
+        <v>185</v>
+      </c>
+      <c r="L25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" t="s">
+        <v>186</v>
+      </c>
+      <c r="L26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" t="s">
+        <v>157</v>
+      </c>
+      <c r="L31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" t="s">
+        <v>143</v>
+      </c>
+      <c r="L32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" t="s">
+        <v>144</v>
+      </c>
+      <c r="J33" t="s">
+        <v>204</v>
+      </c>
+      <c r="L33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" t="s">
+        <v>145</v>
+      </c>
+      <c r="L34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" t="s">
+        <v>159</v>
+      </c>
+      <c r="L35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
+      </c>
+      <c r="L38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+      <c r="L39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" t="s">
+        <v>158</v>
+      </c>
+      <c r="L40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" t="s">
+        <v>161</v>
+      </c>
+      <c r="L41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="J42" t="s">
+        <v>205</v>
+      </c>
+      <c r="L42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F43" t="s">
+        <v>164</v>
+      </c>
+      <c r="L43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" t="s">
+        <v>36</v>
+      </c>
+      <c r="G71" t="s">
+        <v>36</v>
+      </c>
+      <c r="I71" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -891,7 +2003,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -902,7 +2014,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -913,7 +2025,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
@@ -924,7 +2036,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -935,7 +2047,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>129</v>
       </c>
@@ -946,7 +2058,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -957,7 +2069,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -968,7 +2080,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -979,7 +2091,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -989,8 +2101,11 @@
       <c r="D11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +2119,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +2133,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1032,7 +2147,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1046,7 +2161,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1056,8 +2171,11 @@
       <c r="D16" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1067,8 +2185,11 @@
       <c r="D17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1078,8 +2199,11 @@
       <c r="D18" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1090,7 +2214,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1100,8 +2224,11 @@
       <c r="D20" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +2239,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1129,7 +2256,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>126</v>
       </c>
@@ -1140,7 +2267,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1151,7 +2278,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1161,8 +2288,11 @@
       <c r="D25" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1173,7 +2303,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1184,7 +2314,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1195,7 +2325,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>130</v>
       </c>
@@ -1206,7 +2336,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1216,8 +2346,11 @@
       <c r="D30" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1228,23 +2361,29 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
       <c r="C32" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1255,7 +2394,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1265,8 +2404,11 @@
       <c r="D35" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1276,16 +2418,25 @@
       <c r="D36" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
       <c r="B37" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1293,7 +2444,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1301,7 +2452,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1311,8 +2462,11 @@
       <c r="D40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>133</v>
       </c>
@@ -1320,15 +2474,18 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>70</v>
       </c>
@@ -1336,7 +2493,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -1344,7 +2501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1352,17 +2509,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>77</v>
       </c>
@@ -1428,30 +2585,87 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Essentially working version of excel driven hotkeys for TextBlade.
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="347">
   <si>
     <t>a</t>
   </si>
@@ -1151,9 +1151,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys" displayName="HotKeys" ref="A1:M120" totalsRowShown="0">
-  <autoFilter ref="A1:M120"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys" displayName="HotKeys" ref="A1:N120" totalsRowShown="0">
+  <autoFilter ref="A1:N120"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
     <tableColumn id="3" name="Alpha Up"/>
@@ -1167,6 +1167,7 @@
     <tableColumn id="12" name="Media Up"/>
     <tableColumn id="10" name="Green Media Down"/>
     <tableColumn id="13" name="Green Media Up"/>
+    <tableColumn id="14" name="Delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1447,13 +1448,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:N120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43:D44"/>
+      <selection pane="bottomRight" activeCell="N121" sqref="N121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1474,7 @@
     <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1513,8 +1514,11 @@
       <c r="M1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -1548,7 +1552,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1562,7 +1566,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -1576,7 +1580,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1590,7 +1594,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
@@ -1604,7 +1608,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1618,7 +1622,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1646,7 +1650,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -1660,7 +1664,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1674,7 +1678,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>244</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>260</v>
       </c>
@@ -2921,37 +2925,37 @@
         <v>185</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>26</v>
       </c>
@@ -2964,8 +2968,11 @@
       <c r="H119" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N119">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>339</v>
       </c>
@@ -2977,6 +2984,9 @@
       </c>
       <c r="H120" t="s">
         <v>340</v>
+      </c>
+      <c r="N120">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add alternative handling for right side function layers.
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="377">
   <si>
     <t>a</t>
   </si>
@@ -1076,6 +1076,98 @@
   </si>
   <si>
     <t>*x</t>
+  </si>
+  <si>
+    <t>FunctionLowRight Down</t>
+  </si>
+  <si>
+    <t>FunctionLowRight Up</t>
+  </si>
+  <si>
+    <t>FunctionLowRight</t>
+  </si>
+  <si>
+    <t>s
+d</t>
+  </si>
+  <si>
+    <t>a
+s</t>
+  </si>
+  <si>
+    <t>FunctionHighRight</t>
+  </si>
+  <si>
+    <t>FunctionHigh Down</t>
+  </si>
+  <si>
+    <t>FunctionHigh Up</t>
+  </si>
+  <si>
+    <t>FunctionHighRight Down</t>
+  </si>
+  <si>
+    <t>FunctionHighRight Up</t>
+  </si>
+  <si>
+    <t>{F11}</t>
+  </si>
+  <si>
+    <t>{Blind}{F11}</t>
+  </si>
+  <si>
+    <t>{F12}</t>
+  </si>
+  <si>
+    <t>{Blind}{F12}</t>
+  </si>
+  <si>
+    <t>{F13}</t>
+  </si>
+  <si>
+    <t>{Blind}{F13}</t>
+  </si>
+  <si>
+    <t>{F14}</t>
+  </si>
+  <si>
+    <t>{Blind}{F14}</t>
+  </si>
+  <si>
+    <t>{F15}</t>
+  </si>
+  <si>
+    <t>{Blind}{F15}</t>
+  </si>
+  <si>
+    <t>{F16}</t>
+  </si>
+  <si>
+    <t>{Blind}{F16}</t>
+  </si>
+  <si>
+    <t>{F17}</t>
+  </si>
+  <si>
+    <t>{Blind}{F17}</t>
+  </si>
+  <si>
+    <t>{F18}</t>
+  </si>
+  <si>
+    <t>{Blind}{F18}</t>
+  </si>
+  <si>
+    <t>{F19}</t>
+  </si>
+  <si>
+    <t>{Blind}{F19}</t>
+  </si>
+  <si>
+    <t>{F20}</t>
+  </si>
+  <si>
+    <t>{Blind}{F20}</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1225,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1151,9 +1246,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys" displayName="HotKeys" ref="A1:N120" totalsRowShown="0">
-  <autoFilter ref="A1:N120"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys" displayName="HotKeys" ref="A1:T120" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:T120"/>
+  <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
     <tableColumn id="3" name="Alpha Up"/>
@@ -1163,6 +1258,12 @@
     <tableColumn id="7" name="Edit Up"/>
     <tableColumn id="8" name="FunctionLow Down"/>
     <tableColumn id="9" name="FunctionLow Up"/>
+    <tableColumn id="15" name="FunctionLowRight Down"/>
+    <tableColumn id="16" name="FunctionLowRight Up"/>
+    <tableColumn id="20" name="FunctionHigh Down"/>
+    <tableColumn id="19" name="FunctionHigh Up"/>
+    <tableColumn id="18" name="FunctionHighRight Down"/>
+    <tableColumn id="17" name="FunctionHighRight Up"/>
     <tableColumn id="11" name="Media Down"/>
     <tableColumn id="12" name="Media Up"/>
     <tableColumn id="10" name="Green Media Down"/>
@@ -1174,11 +1275,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Layer"/>
-    <tableColumn id="2" name="Keys" dataDxfId="0"/>
+    <tableColumn id="2" name="Keys" dataDxfId="1"/>
     <tableColumn id="3" name="Delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1448,77 +1549,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N120"/>
+  <dimension ref="A1:T120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N121" sqref="N121"/>
+      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1531,11 +1653,11 @@
       <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="L2" t="s">
+      <c r="R2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -1548,11 +1670,11 @@
       <c r="F3" t="s">
         <v>238</v>
       </c>
-      <c r="L3" t="s">
+      <c r="R3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1565,8 +1687,17 @@
       <c r="H4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" t="s">
+        <v>357</v>
+      </c>
+      <c r="N4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -1579,8 +1710,17 @@
       <c r="H5" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L5" t="s">
+        <v>358</v>
+      </c>
+      <c r="N5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1593,8 +1733,17 @@
       <c r="H6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>168</v>
+      </c>
+      <c r="L6" t="s">
+        <v>359</v>
+      </c>
+      <c r="N6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
@@ -1607,8 +1756,17 @@
       <c r="H7" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>256</v>
+      </c>
+      <c r="L7" t="s">
+        <v>360</v>
+      </c>
+      <c r="N7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1621,8 +1779,17 @@
       <c r="H8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>169</v>
+      </c>
+      <c r="L8" t="s">
+        <v>361</v>
+      </c>
+      <c r="N8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -1635,8 +1802,17 @@
       <c r="H9" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>257</v>
+      </c>
+      <c r="L9" t="s">
+        <v>362</v>
+      </c>
+      <c r="N9" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1649,8 +1825,17 @@
       <c r="H10" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>170</v>
+      </c>
+      <c r="L10" t="s">
+        <v>363</v>
+      </c>
+      <c r="N10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -1663,8 +1848,17 @@
       <c r="H11" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>258</v>
+      </c>
+      <c r="L11" t="s">
+        <v>364</v>
+      </c>
+      <c r="N11" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1677,8 +1871,17 @@
       <c r="H12" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>171</v>
+      </c>
+      <c r="L12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>244</v>
       </c>
@@ -1691,8 +1894,17 @@
       <c r="H13" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>259</v>
+      </c>
+      <c r="L13" t="s">
+        <v>366</v>
+      </c>
+      <c r="N13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1700,7 +1912,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1711,7 +1923,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>260</v>
       </c>
@@ -1910,7 +2122,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1921,7 +2133,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>264</v>
       </c>
@@ -1932,7 +2144,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1943,7 +2155,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>265</v>
       </c>
@@ -1954,7 +2166,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1965,7 +2177,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>130</v>
       </c>
@@ -1976,7 +2188,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>209</v>
       </c>
@@ -1987,7 +2199,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>346</v>
       </c>
@@ -1998,7 +2210,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -2009,7 +2221,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -2020,7 +2232,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>341</v>
       </c>
@@ -2031,7 +2243,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>344</v>
       </c>
@@ -2042,7 +2254,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -2053,7 +2265,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>266</v>
       </c>
@@ -2064,7 +2276,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -2080,11 +2292,20 @@
       <c r="H47" t="s">
         <v>173</v>
       </c>
+      <c r="J47" t="s">
+        <v>173</v>
+      </c>
       <c r="L47" t="s">
+        <v>367</v>
+      </c>
+      <c r="N47" t="s">
+        <v>367</v>
+      </c>
+      <c r="R47" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>267</v>
       </c>
@@ -2100,11 +2321,20 @@
       <c r="H48" t="s">
         <v>282</v>
       </c>
+      <c r="J48" t="s">
+        <v>282</v>
+      </c>
       <c r="L48" t="s">
+        <v>368</v>
+      </c>
+      <c r="N48" t="s">
+        <v>368</v>
+      </c>
+      <c r="R48" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -2120,11 +2350,20 @@
       <c r="H49" t="s">
         <v>174</v>
       </c>
+      <c r="J49" t="s">
+        <v>174</v>
+      </c>
       <c r="L49" t="s">
+        <v>369</v>
+      </c>
+      <c r="N49" t="s">
+        <v>369</v>
+      </c>
+      <c r="R49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>268</v>
       </c>
@@ -2140,11 +2379,20 @@
       <c r="H50" t="s">
         <v>286</v>
       </c>
+      <c r="J50" t="s">
+        <v>286</v>
+      </c>
       <c r="L50" t="s">
+        <v>370</v>
+      </c>
+      <c r="N50" t="s">
+        <v>370</v>
+      </c>
+      <c r="R50" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2161,13 +2409,22 @@
         <v>175</v>
       </c>
       <c r="J51" t="s">
+        <v>175</v>
+      </c>
+      <c r="L51" t="s">
+        <v>371</v>
+      </c>
+      <c r="N51" t="s">
+        <v>371</v>
+      </c>
+      <c r="P51" t="s">
         <v>191</v>
       </c>
-      <c r="L51" t="s">
+      <c r="R51" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>269</v>
       </c>
@@ -2184,13 +2441,22 @@
         <v>290</v>
       </c>
       <c r="J52" t="s">
+        <v>290</v>
+      </c>
+      <c r="L52" t="s">
+        <v>372</v>
+      </c>
+      <c r="N52" t="s">
+        <v>372</v>
+      </c>
+      <c r="P52" t="s">
         <v>298</v>
       </c>
-      <c r="L52" t="s">
+      <c r="R52" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -2206,11 +2472,20 @@
       <c r="H53" t="s">
         <v>176</v>
       </c>
+      <c r="J53" t="s">
+        <v>176</v>
+      </c>
       <c r="L53" t="s">
+        <v>373</v>
+      </c>
+      <c r="N53" t="s">
+        <v>373</v>
+      </c>
+      <c r="R53" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>270</v>
       </c>
@@ -2226,11 +2501,20 @@
       <c r="H54" t="s">
         <v>291</v>
       </c>
+      <c r="J54" t="s">
+        <v>291</v>
+      </c>
       <c r="L54" t="s">
+        <v>374</v>
+      </c>
+      <c r="N54" t="s">
+        <v>374</v>
+      </c>
+      <c r="R54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2243,11 +2527,20 @@
       <c r="H55" t="s">
         <v>172</v>
       </c>
+      <c r="J55" t="s">
+        <v>172</v>
+      </c>
       <c r="L55" t="s">
+        <v>375</v>
+      </c>
+      <c r="N55" t="s">
+        <v>375</v>
+      </c>
+      <c r="R55" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>271</v>
       </c>
@@ -2260,11 +2553,20 @@
       <c r="H56" t="s">
         <v>289</v>
       </c>
+      <c r="J56" t="s">
+        <v>289</v>
+      </c>
       <c r="L56" t="s">
+        <v>376</v>
+      </c>
+      <c r="N56" t="s">
+        <v>376</v>
+      </c>
+      <c r="R56" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -2277,11 +2579,11 @@
       <c r="F57" t="s">
         <v>68</v>
       </c>
-      <c r="L57" t="s">
+      <c r="R57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
@@ -2289,7 +2591,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>205</v>
       </c>
@@ -2297,7 +2599,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>207</v>
       </c>
@@ -2310,11 +2612,11 @@
       <c r="F60" t="s">
         <v>208</v>
       </c>
-      <c r="L60" t="s">
+      <c r="R60" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -2330,11 +2632,20 @@
       <c r="H61" t="s">
         <v>68</v>
       </c>
+      <c r="J61" t="s">
+        <v>68</v>
+      </c>
       <c r="L61" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N61" t="s">
+        <v>68</v>
+      </c>
+      <c r="R61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>299</v>
       </c>
@@ -2350,11 +2661,20 @@
       <c r="H62" t="s">
         <v>68</v>
       </c>
+      <c r="J62" t="s">
+        <v>68</v>
+      </c>
       <c r="L62" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N62" t="s">
+        <v>68</v>
+      </c>
+      <c r="R62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -2370,11 +2690,20 @@
       <c r="H63" t="s">
         <v>68</v>
       </c>
+      <c r="J63" t="s">
+        <v>68</v>
+      </c>
       <c r="L63" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N63" t="s">
+        <v>68</v>
+      </c>
+      <c r="R63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>300</v>
       </c>
@@ -2390,11 +2719,20 @@
       <c r="H64" t="s">
         <v>68</v>
       </c>
+      <c r="J64" t="s">
+        <v>68</v>
+      </c>
       <c r="L64" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N64" t="s">
+        <v>68</v>
+      </c>
+      <c r="R64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -2407,11 +2745,11 @@
       <c r="F65" t="s">
         <v>157</v>
       </c>
-      <c r="L65" t="s">
+      <c r="R65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>301</v>
       </c>
@@ -2424,11 +2762,11 @@
       <c r="F66" t="s">
         <v>157</v>
       </c>
-      <c r="L66" t="s">
+      <c r="R66" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -2441,11 +2779,11 @@
       <c r="F67" t="s">
         <v>143</v>
       </c>
-      <c r="L67" t="s">
+      <c r="R67" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>302</v>
       </c>
@@ -2458,11 +2796,11 @@
       <c r="F68" t="s">
         <v>309</v>
       </c>
-      <c r="L68" t="s">
+      <c r="R68" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>25</v>
       </c>
@@ -2475,14 +2813,14 @@
       <c r="F69" t="s">
         <v>144</v>
       </c>
-      <c r="J69" t="s">
+      <c r="P69" t="s">
         <v>194</v>
       </c>
-      <c r="L69" t="s">
+      <c r="R69" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>303</v>
       </c>
@@ -2495,14 +2833,14 @@
       <c r="F70" t="s">
         <v>310</v>
       </c>
-      <c r="J70" t="s">
+      <c r="P70" t="s">
         <v>308</v>
       </c>
-      <c r="L70" t="s">
+      <c r="R70" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -2515,11 +2853,11 @@
       <c r="F71" t="s">
         <v>145</v>
       </c>
-      <c r="L71" t="s">
+      <c r="R71" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>304</v>
       </c>
@@ -2532,11 +2870,11 @@
       <c r="F72" t="s">
         <v>311</v>
       </c>
-      <c r="L72" t="s">
+      <c r="R72" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -2549,11 +2887,11 @@
       <c r="F73" t="s">
         <v>159</v>
       </c>
-      <c r="L73" t="s">
+      <c r="R73" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>133</v>
       </c>
@@ -2561,7 +2899,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>201</v>
       </c>
@@ -2569,7 +2907,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>203</v>
       </c>
@@ -2577,7 +2915,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>35</v>
       </c>
@@ -2587,11 +2925,11 @@
       <c r="F77" t="s">
         <v>37</v>
       </c>
-      <c r="L77" t="s">
+      <c r="R77" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>325</v>
       </c>
@@ -2601,11 +2939,11 @@
       <c r="F78" t="s">
         <v>326</v>
       </c>
-      <c r="L78" t="s">
+      <c r="R78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>27</v>
       </c>
@@ -2615,11 +2953,11 @@
       <c r="F79" t="s">
         <v>37</v>
       </c>
-      <c r="L79" t="s">
+      <c r="R79" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>318</v>
       </c>
@@ -2629,11 +2967,11 @@
       <c r="F80" t="s">
         <v>326</v>
       </c>
-      <c r="L80" t="s">
+      <c r="R80" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -2643,11 +2981,11 @@
       <c r="D81" t="s">
         <v>92</v>
       </c>
-      <c r="L81" t="s">
+      <c r="R81" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>319</v>
       </c>
@@ -2657,11 +2995,11 @@
       <c r="D82" t="s">
         <v>332</v>
       </c>
-      <c r="L82" t="s">
+      <c r="R82" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -2674,11 +3012,11 @@
       <c r="F83" t="s">
         <v>158</v>
       </c>
-      <c r="L83" t="s">
+      <c r="R83" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>320</v>
       </c>
@@ -2691,11 +3029,11 @@
       <c r="F84" t="s">
         <v>158</v>
       </c>
-      <c r="L84" t="s">
+      <c r="R84" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -2708,11 +3046,11 @@
       <c r="F85" t="s">
         <v>161</v>
       </c>
-      <c r="L85" t="s">
+      <c r="R85" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>321</v>
       </c>
@@ -2725,11 +3063,11 @@
       <c r="F86" t="s">
         <v>161</v>
       </c>
-      <c r="L86" t="s">
+      <c r="R86" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>28</v>
       </c>
@@ -2739,14 +3077,14 @@
       <c r="D87" t="s">
         <v>123</v>
       </c>
-      <c r="J87" t="s">
+      <c r="P87" t="s">
         <v>195</v>
       </c>
-      <c r="L87" t="s">
+      <c r="R87" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>322</v>
       </c>
@@ -2756,14 +3094,14 @@
       <c r="D88" t="s">
         <v>335</v>
       </c>
-      <c r="J88" t="s">
+      <c r="P88" t="s">
         <v>338</v>
       </c>
-      <c r="L88" t="s">
+      <c r="R88" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>29</v>
       </c>
@@ -2776,11 +3114,11 @@
       <c r="F89" t="s">
         <v>164</v>
       </c>
-      <c r="L89" t="s">
+      <c r="R89" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>323</v>
       </c>
@@ -2793,11 +3131,11 @@
       <c r="F90" t="s">
         <v>164</v>
       </c>
-      <c r="L90" t="s">
+      <c r="R90" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>30</v>
       </c>
@@ -2811,7 +3149,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>324</v>
       </c>
@@ -2825,22 +3163,22 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>177</v>
       </c>
@@ -2925,37 +3263,37 @@
         <v>185</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>26</v>
       </c>
@@ -2968,11 +3306,20 @@
       <c r="H119" t="s">
         <v>36</v>
       </c>
-      <c r="N119">
+      <c r="J119" t="s">
+        <v>36</v>
+      </c>
+      <c r="L119" t="s">
+        <v>36</v>
+      </c>
+      <c r="N119" t="s">
+        <v>36</v>
+      </c>
+      <c r="T119">
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>339</v>
       </c>
@@ -2985,7 +3332,16 @@
       <c r="H120" t="s">
         <v>340</v>
       </c>
-      <c r="N120">
+      <c r="J120" t="s">
+        <v>340</v>
+      </c>
+      <c r="L120" t="s">
+        <v>340</v>
+      </c>
+      <c r="N120" t="s">
+        <v>340</v>
+      </c>
+      <c r="T120">
         <v>100</v>
       </c>
     </row>
@@ -2995,23 +3351,24 @@
     <hyperlink ref="D20" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3081,6 +3438,22 @@
         <v>60</v>
       </c>
     </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Implement layouts with Colemak added
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Keys" sheetId="4" r:id="rId1"/>
-    <sheet name="Layers" sheetId="3" r:id="rId2"/>
+    <sheet name="Keys.Colemak" sheetId="5" r:id="rId1"/>
+    <sheet name="Keys.QWERTY" sheetId="4" r:id="rId2"/>
+    <sheet name="Layers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="380">
   <si>
     <t>a</t>
   </si>
@@ -1168,6 +1169,15 @@
   </si>
   <si>
     <t>{Blind}{F20}</t>
+  </si>
+  <si>
+    <t>+{r}</t>
+  </si>
+  <si>
+    <t>{O}</t>
+  </si>
+  <si>
+    <t>{Blind}{O}</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1235,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1246,7 +1259,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys" displayName="HotKeys" ref="A1:T120" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T120" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:T120"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
@@ -1275,11 +1288,40 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:T120" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:T120"/>
+  <tableColumns count="20">
+    <tableColumn id="1" name="Hotkey"/>
+    <tableColumn id="2" name="Alpha Down"/>
+    <tableColumn id="3" name="Alpha Up"/>
+    <tableColumn id="4" name="Green Down"/>
+    <tableColumn id="5" name="Green Up"/>
+    <tableColumn id="6" name="Edit Down"/>
+    <tableColumn id="7" name="Edit Up"/>
+    <tableColumn id="8" name="FunctionLow Down"/>
+    <tableColumn id="9" name="FunctionLow Up"/>
+    <tableColumn id="15" name="FunctionLowRight Down"/>
+    <tableColumn id="16" name="FunctionLowRight Up"/>
+    <tableColumn id="20" name="FunctionHigh Down"/>
+    <tableColumn id="19" name="FunctionHigh Up"/>
+    <tableColumn id="18" name="FunctionHighRight Down"/>
+    <tableColumn id="17" name="FunctionHighRight Up"/>
+    <tableColumn id="11" name="Media Down"/>
+    <tableColumn id="12" name="Media Up"/>
+    <tableColumn id="10" name="Green Media Down"/>
+    <tableColumn id="13" name="Green Media Up"/>
+    <tableColumn id="14" name="Delay"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Layer"/>
-    <tableColumn id="2" name="Keys" dataDxfId="1"/>
+    <tableColumn id="2" name="Keys" dataDxfId="0"/>
     <tableColumn id="3" name="Delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1552,10 +1594,10 @@
   <dimension ref="A1:T120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,7 +1813,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
         <v>98</v>
@@ -1794,7 +1836,7 @@
         <v>242</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="D9" t="s">
         <v>252</v>
@@ -1817,7 +1859,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>111</v>
@@ -1840,7 +1882,7 @@
         <v>243</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>297</v>
       </c>
       <c r="D11" t="s">
         <v>253</v>
@@ -1863,7 +1905,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>113</v>
@@ -1886,7 +1928,7 @@
         <v>244</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="D13" t="s">
         <v>254</v>
@@ -1939,7 +1981,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>112</v>
@@ -1956,7 +1998,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>377</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>128</v>
@@ -1967,7 +2009,7 @@
         <v>213</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>215</v>
@@ -1978,7 +2020,7 @@
         <v>216</v>
       </c>
       <c r="B20" t="s">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>217</v>
@@ -1995,7 +2037,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
         <v>97</v>
@@ -2006,7 +2048,7 @@
         <v>129</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D22" t="s">
         <v>125</v>
@@ -2017,7 +2059,7 @@
         <v>223</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>228</v>
@@ -2028,7 +2070,7 @@
         <v>224</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>229</v>
@@ -2039,7 +2081,7 @@
         <v>225</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>230</v>
@@ -2050,7 +2092,7 @@
         <v>226</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>231</v>
@@ -2061,7 +2103,7 @@
         <v>233</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D27" t="s">
         <v>234</v>
@@ -2072,7 +2114,7 @@
         <v>227</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>232</v>
@@ -2083,7 +2125,7 @@
         <v>235</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D29" t="s">
         <v>236</v>
@@ -2094,7 +2136,7 @@
         <v>221</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D30" t="s">
         <v>222</v>
@@ -2105,7 +2147,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
         <v>99</v>
@@ -2116,7 +2158,7 @@
         <v>263</v>
       </c>
       <c r="B32" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="D32" t="s">
         <v>273</v>
@@ -2127,7 +2169,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
         <v>101</v>
@@ -2138,7 +2180,7 @@
         <v>264</v>
       </c>
       <c r="B34" t="s">
-        <v>274</v>
+        <v>220</v>
       </c>
       <c r="D34" t="s">
         <v>275</v>
@@ -2281,7 +2323,7 @@
         <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D47" t="s">
         <v>118</v>
@@ -2310,7 +2352,7 @@
         <v>267</v>
       </c>
       <c r="B48" t="s">
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="D48" t="s">
         <v>281</v>
@@ -2339,7 +2381,7 @@
         <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D49" t="s">
         <v>114</v>
@@ -2368,7 +2410,7 @@
         <v>268</v>
       </c>
       <c r="B50" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
       <c r="D50" t="s">
         <v>284</v>
@@ -2397,7 +2439,7 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D51" t="s">
         <v>102</v>
@@ -2429,7 +2471,7 @@
         <v>269</v>
       </c>
       <c r="B52" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="D52" t="s">
         <v>287</v>
@@ -2461,7 +2503,7 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
         <v>108</v>
@@ -2490,7 +2532,7 @@
         <v>270</v>
       </c>
       <c r="B54" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="D54" t="s">
         <v>288</v>
@@ -2519,7 +2561,7 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D55" t="s">
         <v>109</v>
@@ -2545,7 +2587,7 @@
         <v>271</v>
       </c>
       <c r="B56" t="s">
-        <v>297</v>
+        <v>204</v>
       </c>
       <c r="D56" t="s">
         <v>294</v>
@@ -2771,7 +2813,7 @@
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D67" t="s">
         <v>103</v>
@@ -2788,7 +2830,7 @@
         <v>302</v>
       </c>
       <c r="B68" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="D68" t="s">
         <v>312</v>
@@ -2805,7 +2847,7 @@
         <v>25</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D69" t="s">
         <v>104</v>
@@ -2825,7 +2867,7 @@
         <v>303</v>
       </c>
       <c r="B70" t="s">
-        <v>316</v>
+        <v>247</v>
       </c>
       <c r="D70" t="s">
         <v>313</v>
@@ -2845,7 +2887,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D71" t="s">
         <v>105</v>
@@ -2862,7 +2904,7 @@
         <v>304</v>
       </c>
       <c r="B72" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="D72" t="s">
         <v>314</v>
@@ -2879,7 +2921,7 @@
         <v>34</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D73" t="s">
         <v>120</v>
@@ -2896,7 +2938,7 @@
         <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>134</v>
+        <v>378</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
@@ -2904,7 +2946,7 @@
         <v>201</v>
       </c>
       <c r="B75" t="s">
-        <v>202</v>
+        <v>379</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
@@ -2912,7 +2954,7 @@
         <v>203</v>
       </c>
       <c r="B76" t="s">
-        <v>204</v>
+        <v>296</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
@@ -3004,7 +3046,7 @@
         <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D83" t="s">
         <v>107</v>
@@ -3021,7 +3063,7 @@
         <v>320</v>
       </c>
       <c r="B84" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="D84" t="s">
         <v>333</v>
@@ -3359,6 +3401,1817 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T120"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" t="s">
+        <v>238</v>
+      </c>
+      <c r="R3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" t="s">
+        <v>357</v>
+      </c>
+      <c r="N4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5" t="s">
+        <v>255</v>
+      </c>
+      <c r="J5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L5" t="s">
+        <v>358</v>
+      </c>
+      <c r="N5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" t="s">
+        <v>168</v>
+      </c>
+      <c r="L6" t="s">
+        <v>359</v>
+      </c>
+      <c r="N6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" t="s">
+        <v>251</v>
+      </c>
+      <c r="H7" t="s">
+        <v>256</v>
+      </c>
+      <c r="J7" t="s">
+        <v>256</v>
+      </c>
+      <c r="L7" t="s">
+        <v>360</v>
+      </c>
+      <c r="N7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" t="s">
+        <v>169</v>
+      </c>
+      <c r="L8" t="s">
+        <v>361</v>
+      </c>
+      <c r="N8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H9" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" t="s">
+        <v>257</v>
+      </c>
+      <c r="L9" t="s">
+        <v>362</v>
+      </c>
+      <c r="N9" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" t="s">
+        <v>170</v>
+      </c>
+      <c r="L10" t="s">
+        <v>363</v>
+      </c>
+      <c r="N10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" t="s">
+        <v>253</v>
+      </c>
+      <c r="H11" t="s">
+        <v>258</v>
+      </c>
+      <c r="J11" t="s">
+        <v>258</v>
+      </c>
+      <c r="L11" t="s">
+        <v>364</v>
+      </c>
+      <c r="N11" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H12" t="s">
+        <v>171</v>
+      </c>
+      <c r="J12" t="s">
+        <v>171</v>
+      </c>
+      <c r="L12" t="s">
+        <v>365</v>
+      </c>
+      <c r="N12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" t="s">
+        <v>254</v>
+      </c>
+      <c r="H13" t="s">
+        <v>259</v>
+      </c>
+      <c r="J13" t="s">
+        <v>259</v>
+      </c>
+      <c r="L13" t="s">
+        <v>366</v>
+      </c>
+      <c r="N13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20" t="s">
+        <v>218</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" t="s">
+        <v>220</v>
+      </c>
+      <c r="D30" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>263</v>
+      </c>
+      <c r="B32" t="s">
+        <v>272</v>
+      </c>
+      <c r="D32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>264</v>
+      </c>
+      <c r="B34" t="s">
+        <v>274</v>
+      </c>
+      <c r="D34" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>265</v>
+      </c>
+      <c r="B36" t="s">
+        <v>276</v>
+      </c>
+      <c r="D36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>346</v>
+      </c>
+      <c r="B40" t="s">
+        <v>210</v>
+      </c>
+      <c r="D40" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D43" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>344</v>
+      </c>
+      <c r="B44" t="s">
+        <v>342</v>
+      </c>
+      <c r="D44" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>266</v>
+      </c>
+      <c r="B46" t="s">
+        <v>278</v>
+      </c>
+      <c r="D46" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" t="s">
+        <v>156</v>
+      </c>
+      <c r="H47" t="s">
+        <v>173</v>
+      </c>
+      <c r="J47" t="s">
+        <v>173</v>
+      </c>
+      <c r="L47" t="s">
+        <v>367</v>
+      </c>
+      <c r="N47" t="s">
+        <v>367</v>
+      </c>
+      <c r="R47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>267</v>
+      </c>
+      <c r="B48" t="s">
+        <v>280</v>
+      </c>
+      <c r="D48" t="s">
+        <v>281</v>
+      </c>
+      <c r="F48" t="s">
+        <v>156</v>
+      </c>
+      <c r="H48" t="s">
+        <v>282</v>
+      </c>
+      <c r="J48" t="s">
+        <v>282</v>
+      </c>
+      <c r="L48" t="s">
+        <v>368</v>
+      </c>
+      <c r="N48" t="s">
+        <v>368</v>
+      </c>
+      <c r="R48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" t="s">
+        <v>162</v>
+      </c>
+      <c r="H49" t="s">
+        <v>174</v>
+      </c>
+      <c r="J49" t="s">
+        <v>174</v>
+      </c>
+      <c r="L49" t="s">
+        <v>369</v>
+      </c>
+      <c r="N49" t="s">
+        <v>369</v>
+      </c>
+      <c r="R49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>268</v>
+      </c>
+      <c r="B50" t="s">
+        <v>283</v>
+      </c>
+      <c r="D50" t="s">
+        <v>284</v>
+      </c>
+      <c r="F50" t="s">
+        <v>285</v>
+      </c>
+      <c r="H50" t="s">
+        <v>286</v>
+      </c>
+      <c r="J50" t="s">
+        <v>286</v>
+      </c>
+      <c r="L50" t="s">
+        <v>370</v>
+      </c>
+      <c r="N50" t="s">
+        <v>370</v>
+      </c>
+      <c r="R50" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" t="s">
+        <v>142</v>
+      </c>
+      <c r="H51" t="s">
+        <v>175</v>
+      </c>
+      <c r="J51" t="s">
+        <v>175</v>
+      </c>
+      <c r="L51" t="s">
+        <v>371</v>
+      </c>
+      <c r="N51" t="s">
+        <v>371</v>
+      </c>
+      <c r="P51" t="s">
+        <v>191</v>
+      </c>
+      <c r="R51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>269</v>
+      </c>
+      <c r="B52" t="s">
+        <v>295</v>
+      </c>
+      <c r="D52" t="s">
+        <v>287</v>
+      </c>
+      <c r="F52" t="s">
+        <v>292</v>
+      </c>
+      <c r="H52" t="s">
+        <v>290</v>
+      </c>
+      <c r="J52" t="s">
+        <v>290</v>
+      </c>
+      <c r="L52" t="s">
+        <v>372</v>
+      </c>
+      <c r="N52" t="s">
+        <v>372</v>
+      </c>
+      <c r="P52" t="s">
+        <v>298</v>
+      </c>
+      <c r="R52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" t="s">
+        <v>163</v>
+      </c>
+      <c r="H53" t="s">
+        <v>176</v>
+      </c>
+      <c r="J53" t="s">
+        <v>176</v>
+      </c>
+      <c r="L53" t="s">
+        <v>373</v>
+      </c>
+      <c r="N53" t="s">
+        <v>373</v>
+      </c>
+      <c r="R53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>270</v>
+      </c>
+      <c r="B54" t="s">
+        <v>296</v>
+      </c>
+      <c r="D54" t="s">
+        <v>288</v>
+      </c>
+      <c r="F54" t="s">
+        <v>293</v>
+      </c>
+      <c r="H54" t="s">
+        <v>291</v>
+      </c>
+      <c r="J54" t="s">
+        <v>291</v>
+      </c>
+      <c r="L54" t="s">
+        <v>374</v>
+      </c>
+      <c r="N54" t="s">
+        <v>374</v>
+      </c>
+      <c r="R54" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" t="s">
+        <v>109</v>
+      </c>
+      <c r="H55" t="s">
+        <v>172</v>
+      </c>
+      <c r="J55" t="s">
+        <v>172</v>
+      </c>
+      <c r="L55" t="s">
+        <v>375</v>
+      </c>
+      <c r="N55" t="s">
+        <v>375</v>
+      </c>
+      <c r="R55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>271</v>
+      </c>
+      <c r="B56" t="s">
+        <v>297</v>
+      </c>
+      <c r="D56" t="s">
+        <v>294</v>
+      </c>
+      <c r="H56" t="s">
+        <v>289</v>
+      </c>
+      <c r="J56" t="s">
+        <v>289</v>
+      </c>
+      <c r="L56" t="s">
+        <v>376</v>
+      </c>
+      <c r="N56" t="s">
+        <v>376</v>
+      </c>
+      <c r="R56" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" t="s">
+        <v>68</v>
+      </c>
+      <c r="R57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B59" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>207</v>
+      </c>
+      <c r="B60" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" t="s">
+        <v>206</v>
+      </c>
+      <c r="F60" t="s">
+        <v>208</v>
+      </c>
+      <c r="R60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" t="s">
+        <v>71</v>
+      </c>
+      <c r="F61" t="s">
+        <v>68</v>
+      </c>
+      <c r="H61" t="s">
+        <v>68</v>
+      </c>
+      <c r="J61" t="s">
+        <v>68</v>
+      </c>
+      <c r="L61" t="s">
+        <v>68</v>
+      </c>
+      <c r="N61" t="s">
+        <v>68</v>
+      </c>
+      <c r="R61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>299</v>
+      </c>
+      <c r="B62" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" t="s">
+        <v>71</v>
+      </c>
+      <c r="F62" t="s">
+        <v>68</v>
+      </c>
+      <c r="H62" t="s">
+        <v>68</v>
+      </c>
+      <c r="J62" t="s">
+        <v>68</v>
+      </c>
+      <c r="L62" t="s">
+        <v>68</v>
+      </c>
+      <c r="N62" t="s">
+        <v>68</v>
+      </c>
+      <c r="R62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" t="s">
+        <v>71</v>
+      </c>
+      <c r="F63" t="s">
+        <v>68</v>
+      </c>
+      <c r="H63" t="s">
+        <v>68</v>
+      </c>
+      <c r="J63" t="s">
+        <v>68</v>
+      </c>
+      <c r="L63" t="s">
+        <v>68</v>
+      </c>
+      <c r="N63" t="s">
+        <v>68</v>
+      </c>
+      <c r="R63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>300</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" t="s">
+        <v>68</v>
+      </c>
+      <c r="H64" t="s">
+        <v>68</v>
+      </c>
+      <c r="J64" t="s">
+        <v>68</v>
+      </c>
+      <c r="L64" t="s">
+        <v>68</v>
+      </c>
+      <c r="N64" t="s">
+        <v>68</v>
+      </c>
+      <c r="R64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" t="s">
+        <v>100</v>
+      </c>
+      <c r="F65" t="s">
+        <v>157</v>
+      </c>
+      <c r="R65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>301</v>
+      </c>
+      <c r="B66" t="s">
+        <v>305</v>
+      </c>
+      <c r="D66" t="s">
+        <v>306</v>
+      </c>
+      <c r="F66" t="s">
+        <v>157</v>
+      </c>
+      <c r="R66" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" t="s">
+        <v>103</v>
+      </c>
+      <c r="F67" t="s">
+        <v>143</v>
+      </c>
+      <c r="R67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>302</v>
+      </c>
+      <c r="B68" t="s">
+        <v>315</v>
+      </c>
+      <c r="D68" t="s">
+        <v>312</v>
+      </c>
+      <c r="F68" t="s">
+        <v>309</v>
+      </c>
+      <c r="R68" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69" t="s">
+        <v>49</v>
+      </c>
+      <c r="D69" t="s">
+        <v>104</v>
+      </c>
+      <c r="F69" t="s">
+        <v>144</v>
+      </c>
+      <c r="P69" t="s">
+        <v>194</v>
+      </c>
+      <c r="R69" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>303</v>
+      </c>
+      <c r="B70" t="s">
+        <v>316</v>
+      </c>
+      <c r="D70" t="s">
+        <v>313</v>
+      </c>
+      <c r="F70" t="s">
+        <v>310</v>
+      </c>
+      <c r="P70" t="s">
+        <v>308</v>
+      </c>
+      <c r="R70" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" t="s">
+        <v>105</v>
+      </c>
+      <c r="F71" t="s">
+        <v>145</v>
+      </c>
+      <c r="R71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>304</v>
+      </c>
+      <c r="B72" t="s">
+        <v>317</v>
+      </c>
+      <c r="D72" t="s">
+        <v>314</v>
+      </c>
+      <c r="F72" t="s">
+        <v>311</v>
+      </c>
+      <c r="R72" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" t="s">
+        <v>69</v>
+      </c>
+      <c r="D73" t="s">
+        <v>120</v>
+      </c>
+      <c r="F73" t="s">
+        <v>159</v>
+      </c>
+      <c r="R73" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B75" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B76" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F77" t="s">
+        <v>37</v>
+      </c>
+      <c r="R77" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F78" t="s">
+        <v>326</v>
+      </c>
+      <c r="R78" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79" t="s">
+        <v>37</v>
+      </c>
+      <c r="F79" t="s">
+        <v>37</v>
+      </c>
+      <c r="R79" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>318</v>
+      </c>
+      <c r="B80" t="s">
+        <v>326</v>
+      </c>
+      <c r="F80" t="s">
+        <v>326</v>
+      </c>
+      <c r="R80" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81" t="s">
+        <v>92</v>
+      </c>
+      <c r="R81" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>319</v>
+      </c>
+      <c r="B82" t="s">
+        <v>327</v>
+      </c>
+      <c r="D82" t="s">
+        <v>332</v>
+      </c>
+      <c r="R82" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" t="s">
+        <v>52</v>
+      </c>
+      <c r="D83" t="s">
+        <v>107</v>
+      </c>
+      <c r="F83" t="s">
+        <v>158</v>
+      </c>
+      <c r="R83" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>320</v>
+      </c>
+      <c r="B84" t="s">
+        <v>328</v>
+      </c>
+      <c r="D84" t="s">
+        <v>333</v>
+      </c>
+      <c r="F84" t="s">
+        <v>158</v>
+      </c>
+      <c r="R84" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" t="s">
+        <v>106</v>
+      </c>
+      <c r="F85" t="s">
+        <v>161</v>
+      </c>
+      <c r="R85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>321</v>
+      </c>
+      <c r="B86" t="s">
+        <v>329</v>
+      </c>
+      <c r="D86" t="s">
+        <v>334</v>
+      </c>
+      <c r="F86" t="s">
+        <v>161</v>
+      </c>
+      <c r="R86" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" t="s">
+        <v>65</v>
+      </c>
+      <c r="D87" t="s">
+        <v>123</v>
+      </c>
+      <c r="P87" t="s">
+        <v>195</v>
+      </c>
+      <c r="R87" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>322</v>
+      </c>
+      <c r="B88" t="s">
+        <v>330</v>
+      </c>
+      <c r="D88" t="s">
+        <v>335</v>
+      </c>
+      <c r="P88" t="s">
+        <v>338</v>
+      </c>
+      <c r="R88" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>29</v>
+      </c>
+      <c r="B89" t="s">
+        <v>66</v>
+      </c>
+      <c r="D89" t="s">
+        <v>121</v>
+      </c>
+      <c r="F89" t="s">
+        <v>164</v>
+      </c>
+      <c r="R89" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>323</v>
+      </c>
+      <c r="B90" t="s">
+        <v>307</v>
+      </c>
+      <c r="D90" t="s">
+        <v>336</v>
+      </c>
+      <c r="F90" t="s">
+        <v>164</v>
+      </c>
+      <c r="R90" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>30</v>
+      </c>
+      <c r="B91" t="s">
+        <v>67</v>
+      </c>
+      <c r="D91" t="s">
+        <v>122</v>
+      </c>
+      <c r="F91" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>324</v>
+      </c>
+      <c r="B92" t="s">
+        <v>331</v>
+      </c>
+      <c r="D92" t="s">
+        <v>337</v>
+      </c>
+      <c r="F92" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119" t="s">
+        <v>36</v>
+      </c>
+      <c r="F119" t="s">
+        <v>36</v>
+      </c>
+      <c r="H119" t="s">
+        <v>36</v>
+      </c>
+      <c r="J119" t="s">
+        <v>36</v>
+      </c>
+      <c r="L119" t="s">
+        <v>36</v>
+      </c>
+      <c r="N119" t="s">
+        <v>36</v>
+      </c>
+      <c r="T119">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>339</v>
+      </c>
+      <c r="B120" t="s">
+        <v>340</v>
+      </c>
+      <c r="F120" t="s">
+        <v>340</v>
+      </c>
+      <c r="H120" t="s">
+        <v>340</v>
+      </c>
+      <c r="J120" t="s">
+        <v>340</v>
+      </c>
+      <c r="L120" t="s">
+        <v>340</v>
+      </c>
+      <c r="N120" t="s">
+        <v>340</v>
+      </c>
+      <c r="T120">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1"/>
+    <hyperlink ref="D20" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix Colemak layout for quote character
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="382">
   <si>
     <t>a</t>
   </si>
@@ -1178,6 +1178,12 @@
   </si>
   <si>
     <t>{Blind}{O}</t>
+  </si>
+  <si>
+    <t>+p</t>
+  </si>
+  <si>
+    <t>+*p</t>
   </si>
 </sst>
 </file>
@@ -1259,8 +1265,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T120" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:T120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T122" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:T122"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
@@ -1591,13 +1597,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T120"/>
+  <dimension ref="A1:T122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2583,11 +2589,11 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>271</v>
+      <c r="A56" s="1" t="s">
+        <v>380</v>
       </c>
       <c r="B56" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
       <c r="D56" t="s">
         <v>294</v>
@@ -2609,108 +2615,66 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>271</v>
+      </c>
+      <c r="B58" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>31</v>
       </c>
-      <c r="B57" t="s">
-        <v>68</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" t="s">
         <v>71</v>
       </c>
-      <c r="F57" t="s">
-        <v>68</v>
-      </c>
-      <c r="R57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="F59" t="s">
+        <v>68</v>
+      </c>
+      <c r="R59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>207</v>
-      </c>
-      <c r="B60" t="s">
-        <v>208</v>
-      </c>
-      <c r="D60" t="s">
-        <v>206</v>
-      </c>
-      <c r="F60" t="s">
-        <v>208</v>
-      </c>
-      <c r="R60" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" t="s">
-        <v>68</v>
-      </c>
-      <c r="D61" t="s">
-        <v>71</v>
-      </c>
-      <c r="F61" t="s">
-        <v>68</v>
-      </c>
-      <c r="H61" t="s">
-        <v>68</v>
-      </c>
-      <c r="J61" t="s">
-        <v>68</v>
-      </c>
-      <c r="L61" t="s">
-        <v>68</v>
-      </c>
-      <c r="N61" t="s">
-        <v>68</v>
-      </c>
-      <c r="R61" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>299</v>
+        <v>207</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>208</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
+        <v>206</v>
       </c>
       <c r="F62" t="s">
-        <v>68</v>
-      </c>
-      <c r="H62" t="s">
-        <v>68</v>
-      </c>
-      <c r="J62" t="s">
-        <v>68</v>
-      </c>
-      <c r="L62" t="s">
-        <v>68</v>
-      </c>
-      <c r="N62" t="s">
-        <v>68</v>
+        <v>208</v>
       </c>
       <c r="R62" t="s">
         <v>68</v>
@@ -2718,7 +2682,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B63" t="s">
         <v>68</v>
@@ -2747,7 +2711,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B64" t="s">
         <v>68</v>
@@ -2776,220 +2740,250 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B65" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D65" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="F65" t="s">
-        <v>157</v>
+        <v>68</v>
+      </c>
+      <c r="H65" t="s">
+        <v>68</v>
+      </c>
+      <c r="J65" t="s">
+        <v>68</v>
+      </c>
+      <c r="L65" t="s">
+        <v>68</v>
+      </c>
+      <c r="N65" t="s">
+        <v>68</v>
       </c>
       <c r="R65" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B66" t="s">
-        <v>305</v>
+        <v>68</v>
       </c>
       <c r="D66" t="s">
-        <v>306</v>
+        <v>71</v>
       </c>
       <c r="F66" t="s">
-        <v>157</v>
+        <v>68</v>
+      </c>
+      <c r="H66" t="s">
+        <v>68</v>
+      </c>
+      <c r="J66" t="s">
+        <v>68</v>
+      </c>
+      <c r="L66" t="s">
+        <v>68</v>
+      </c>
+      <c r="N66" t="s">
+        <v>68</v>
       </c>
       <c r="R66" t="s">
-        <v>307</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D67" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F67" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="R67" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B68" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="D68" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F68" t="s">
-        <v>309</v>
+        <v>157</v>
       </c>
       <c r="R68" t="s">
-        <v>253</v>
+        <v>307</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F69" t="s">
-        <v>144</v>
-      </c>
-      <c r="P69" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="R69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B70" t="s">
-        <v>247</v>
+        <v>328</v>
       </c>
       <c r="D70" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F70" t="s">
-        <v>310</v>
-      </c>
-      <c r="P70" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="R70" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F71" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="P71" t="s">
+        <v>194</v>
       </c>
       <c r="R71" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B72" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
       <c r="D72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F72" t="s">
-        <v>311</v>
+        <v>310</v>
+      </c>
+      <c r="P72" t="s">
+        <v>308</v>
       </c>
       <c r="R72" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" t="s">
+        <v>105</v>
+      </c>
+      <c r="F73" t="s">
+        <v>145</v>
+      </c>
+      <c r="R73" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>304</v>
+      </c>
+      <c r="B74" t="s">
+        <v>295</v>
+      </c>
+      <c r="D74" t="s">
+        <v>314</v>
+      </c>
+      <c r="F74" t="s">
+        <v>311</v>
+      </c>
+      <c r="R74" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>34</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B75" t="s">
         <v>53</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D75" t="s">
         <v>120</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F75" t="s">
         <v>159</v>
       </c>
-      <c r="R73" t="s">
+      <c r="R75" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B74" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B75" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
       <c r="B76" t="s">
-        <v>296</v>
+        <v>378</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F77" t="s">
-        <v>37</v>
-      </c>
-      <c r="R77" t="s">
-        <v>37</v>
+        <v>201</v>
+      </c>
+      <c r="B77" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F78" t="s">
-        <v>326</v>
-      </c>
-      <c r="R78" t="s">
-        <v>326</v>
+        <v>203</v>
+      </c>
+      <c r="B78" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>27</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="A79" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F79" t="s">
@@ -3000,10 +2994,10 @@
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>318</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="A80" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F80" t="s">
@@ -3015,375 +3009,403 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B81" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81" t="s">
-        <v>92</v>
+        <v>37</v>
+      </c>
+      <c r="F81" t="s">
+        <v>37</v>
       </c>
       <c r="R81" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B82" t="s">
-        <v>327</v>
-      </c>
-      <c r="D82" t="s">
-        <v>332</v>
+        <v>326</v>
+      </c>
+      <c r="F82" t="s">
+        <v>326</v>
       </c>
       <c r="R82" t="s">
-        <v>294</v>
+        <v>326</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D83" t="s">
-        <v>107</v>
-      </c>
-      <c r="F83" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="R83" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B84" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="D84" t="s">
-        <v>333</v>
-      </c>
-      <c r="F84" t="s">
-        <v>158</v>
+        <v>332</v>
       </c>
       <c r="R84" t="s">
-        <v>250</v>
+        <v>294</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B85" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D85" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F85" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R85" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B86" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="D86" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F86" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R86" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D87" t="s">
-        <v>123</v>
-      </c>
-      <c r="P87" t="s">
-        <v>195</v>
+        <v>106</v>
+      </c>
+      <c r="F87" t="s">
+        <v>161</v>
       </c>
       <c r="R87" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B88" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D88" t="s">
-        <v>335</v>
-      </c>
-      <c r="P88" t="s">
-        <v>338</v>
+        <v>334</v>
+      </c>
+      <c r="F88" t="s">
+        <v>161</v>
       </c>
       <c r="R88" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B89" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D89" t="s">
-        <v>121</v>
-      </c>
-      <c r="F89" t="s">
-        <v>164</v>
+        <v>123</v>
+      </c>
+      <c r="P89" t="s">
+        <v>195</v>
       </c>
       <c r="R89" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B90" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="D90" t="s">
-        <v>336</v>
-      </c>
-      <c r="F90" t="s">
-        <v>164</v>
+        <v>335</v>
+      </c>
+      <c r="P90" t="s">
+        <v>338</v>
       </c>
       <c r="R90" t="s">
-        <v>331</v>
+        <v>252</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D91" t="s">
+        <v>121</v>
+      </c>
+      <c r="F91" t="s">
+        <v>164</v>
+      </c>
+      <c r="R91" t="s">
         <v>67</v>
-      </c>
-      <c r="D91" t="s">
-        <v>122</v>
-      </c>
-      <c r="F91" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B92" t="s">
+        <v>307</v>
+      </c>
+      <c r="D92" t="s">
+        <v>336</v>
+      </c>
+      <c r="F92" t="s">
+        <v>164</v>
+      </c>
+      <c r="R92" t="s">
         <v>331</v>
-      </c>
-      <c r="D92" t="s">
-        <v>337</v>
-      </c>
-      <c r="F92" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>30</v>
+      </c>
+      <c r="B93" t="s">
+        <v>67</v>
+      </c>
+      <c r="D93" t="s">
+        <v>122</v>
+      </c>
+      <c r="F93" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>324</v>
+      </c>
+      <c r="B94" t="s">
+        <v>331</v>
+      </c>
+      <c r="D94" t="s">
+        <v>337</v>
+      </c>
+      <c r="F94" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>26</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B121" t="s">
         <v>36</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F121" t="s">
         <v>36</v>
       </c>
-      <c r="H119" t="s">
+      <c r="H121" t="s">
         <v>36</v>
       </c>
-      <c r="J119" t="s">
+      <c r="J121" t="s">
         <v>36</v>
       </c>
-      <c r="L119" t="s">
+      <c r="L121" t="s">
         <v>36</v>
       </c>
-      <c r="N119" t="s">
+      <c r="N121" t="s">
         <v>36</v>
       </c>
-      <c r="T119">
+      <c r="T121">
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>339</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B122" t="s">
         <v>340</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F122" t="s">
         <v>340</v>
       </c>
-      <c r="H120" t="s">
+      <c r="H122" t="s">
         <v>340</v>
       </c>
-      <c r="J120" t="s">
+      <c r="J122" t="s">
         <v>340</v>
       </c>
-      <c r="L120" t="s">
+      <c r="L122" t="s">
         <v>340</v>
       </c>
-      <c r="N120" t="s">
+      <c r="N122" t="s">
         <v>340</v>
       </c>
-      <c r="T120">
+      <c r="T122">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add DVORAK and fix issue with quote key
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Keys.Colemak" sheetId="5" r:id="rId1"/>
-    <sheet name="Keys.QWERTY" sheetId="4" r:id="rId2"/>
-    <sheet name="Layers" sheetId="3" r:id="rId3"/>
+    <sheet name="Keys.DVORAK" sheetId="6" r:id="rId1"/>
+    <sheet name="Keys.Colemak" sheetId="5" r:id="rId2"/>
+    <sheet name="Keys.QWERTY" sheetId="4" r:id="rId3"/>
+    <sheet name="Layers" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="394">
   <si>
     <t>a</t>
   </si>
@@ -1184,6 +1185,42 @@
   </si>
   <si>
     <t>+*p</t>
+  </si>
+  <si>
+    <t>+q</t>
+  </si>
+  <si>
+    <t>+*q</t>
+  </si>
+  <si>
+    <t>+w</t>
+  </si>
+  <si>
+    <t>+*w</t>
+  </si>
+  <si>
+    <t>+e</t>
+  </si>
+  <si>
+    <t>+*e</t>
+  </si>
+  <si>
+    <t>+{o}</t>
+  </si>
+  <si>
+    <t>+{e}</t>
+  </si>
+  <si>
+    <t>+z</t>
+  </si>
+  <si>
+    <t>+*z</t>
+  </si>
+  <si>
+    <t>+{q}</t>
+  </si>
+  <si>
+    <t>+{j}</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1278,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1265,7 +1305,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T122" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HotKeys.DVORAK" displayName="HotKeys.DVORAK" ref="A1:T128" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:T128"/>
+  <tableColumns count="20">
+    <tableColumn id="1" name="Hotkey"/>
+    <tableColumn id="2" name="Alpha Down"/>
+    <tableColumn id="3" name="Alpha Up"/>
+    <tableColumn id="4" name="Green Down"/>
+    <tableColumn id="5" name="Green Up"/>
+    <tableColumn id="6" name="Edit Down"/>
+    <tableColumn id="7" name="Edit Up"/>
+    <tableColumn id="8" name="FunctionLow Down"/>
+    <tableColumn id="9" name="FunctionLow Up"/>
+    <tableColumn id="15" name="FunctionLowRight Down"/>
+    <tableColumn id="16" name="FunctionLowRight Up"/>
+    <tableColumn id="20" name="FunctionHigh Down"/>
+    <tableColumn id="19" name="FunctionHigh Up"/>
+    <tableColumn id="18" name="FunctionHighRight Down"/>
+    <tableColumn id="17" name="FunctionHighRight Up"/>
+    <tableColumn id="11" name="Media Down"/>
+    <tableColumn id="12" name="Media Up"/>
+    <tableColumn id="10" name="Green Media Down"/>
+    <tableColumn id="13" name="Green Media Up"/>
+    <tableColumn id="14" name="Delay"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T122" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:T122"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
@@ -1293,8 +1362,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:T120" totalsRowShown="0" headerRowDxfId="1">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:T120" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:T120"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
@@ -1322,12 +1391,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Layer"/>
-    <tableColumn id="2" name="Keys" dataDxfId="0"/>
+    <tableColumn id="2" name="Keys" dataDxfId="1"/>
     <tableColumn id="3" name="Delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1597,13 +1666,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T122"/>
+  <dimension ref="A1:T128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomRight" activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,6 +1796,1977 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" t="s">
+        <v>357</v>
+      </c>
+      <c r="N4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" t="s">
+        <v>255</v>
+      </c>
+      <c r="J5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L5" t="s">
+        <v>358</v>
+      </c>
+      <c r="N5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" t="s">
+        <v>250</v>
+      </c>
+      <c r="H6" t="s">
+        <v>255</v>
+      </c>
+      <c r="J6" t="s">
+        <v>255</v>
+      </c>
+      <c r="L6" t="s">
+        <v>358</v>
+      </c>
+      <c r="N6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" t="s">
+        <v>250</v>
+      </c>
+      <c r="H7" t="s">
+        <v>255</v>
+      </c>
+      <c r="J7" t="s">
+        <v>255</v>
+      </c>
+      <c r="L7" t="s">
+        <v>358</v>
+      </c>
+      <c r="N7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L8" t="s">
+        <v>359</v>
+      </c>
+      <c r="N8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" t="s">
+        <v>330</v>
+      </c>
+      <c r="D9" t="s">
+        <v>251</v>
+      </c>
+      <c r="H9" t="s">
+        <v>256</v>
+      </c>
+      <c r="J9" t="s">
+        <v>256</v>
+      </c>
+      <c r="L9" t="s">
+        <v>360</v>
+      </c>
+      <c r="N9" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B10" t="s">
+        <v>330</v>
+      </c>
+      <c r="D10" t="s">
+        <v>251</v>
+      </c>
+      <c r="H10" t="s">
+        <v>256</v>
+      </c>
+      <c r="J10" t="s">
+        <v>256</v>
+      </c>
+      <c r="L10" t="s">
+        <v>360</v>
+      </c>
+      <c r="N10" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" t="s">
+        <v>251</v>
+      </c>
+      <c r="H11" t="s">
+        <v>256</v>
+      </c>
+      <c r="J11" t="s">
+        <v>256</v>
+      </c>
+      <c r="L11" t="s">
+        <v>360</v>
+      </c>
+      <c r="N11" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" t="s">
+        <v>169</v>
+      </c>
+      <c r="J12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L12" t="s">
+        <v>361</v>
+      </c>
+      <c r="N12" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D13" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" t="s">
+        <v>257</v>
+      </c>
+      <c r="J13" t="s">
+        <v>257</v>
+      </c>
+      <c r="L13" t="s">
+        <v>362</v>
+      </c>
+      <c r="N13" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D14" t="s">
+        <v>252</v>
+      </c>
+      <c r="H14" t="s">
+        <v>257</v>
+      </c>
+      <c r="J14" t="s">
+        <v>257</v>
+      </c>
+      <c r="L14" t="s">
+        <v>362</v>
+      </c>
+      <c r="N14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B15" t="s">
+        <v>307</v>
+      </c>
+      <c r="D15" t="s">
+        <v>252</v>
+      </c>
+      <c r="H15" t="s">
+        <v>257</v>
+      </c>
+      <c r="J15" t="s">
+        <v>257</v>
+      </c>
+      <c r="L15" t="s">
+        <v>362</v>
+      </c>
+      <c r="N15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" t="s">
+        <v>170</v>
+      </c>
+      <c r="L16" t="s">
+        <v>363</v>
+      </c>
+      <c r="N16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B17" t="s">
+        <v>297</v>
+      </c>
+      <c r="D17" t="s">
+        <v>253</v>
+      </c>
+      <c r="H17" t="s">
+        <v>258</v>
+      </c>
+      <c r="J17" t="s">
+        <v>258</v>
+      </c>
+      <c r="L17" t="s">
+        <v>364</v>
+      </c>
+      <c r="N17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" t="s">
+        <v>171</v>
+      </c>
+      <c r="J18" t="s">
+        <v>171</v>
+      </c>
+      <c r="L18" t="s">
+        <v>365</v>
+      </c>
+      <c r="N18" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H19" t="s">
+        <v>259</v>
+      </c>
+      <c r="J19" t="s">
+        <v>259</v>
+      </c>
+      <c r="L19" t="s">
+        <v>366</v>
+      </c>
+      <c r="N19" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>260</v>
+      </c>
+      <c r="B22" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" t="s">
+        <v>140</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B26" t="s">
+        <v>296</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F26" t="s">
+        <v>218</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D35" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>221</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D36" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>263</v>
+      </c>
+      <c r="B38" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B40" t="s">
+        <v>295</v>
+      </c>
+      <c r="D40" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B42" t="s">
+        <v>335</v>
+      </c>
+      <c r="D42" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B43" t="s">
+        <v>335</v>
+      </c>
+      <c r="D43" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>265</v>
+      </c>
+      <c r="B44" t="s">
+        <v>335</v>
+      </c>
+      <c r="D44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D47" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>346</v>
+      </c>
+      <c r="B48" t="s">
+        <v>245</v>
+      </c>
+      <c r="D48" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D51" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>344</v>
+      </c>
+      <c r="B52" t="s">
+        <v>315</v>
+      </c>
+      <c r="D52" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>266</v>
+      </c>
+      <c r="B54" t="s">
+        <v>316</v>
+      </c>
+      <c r="D54" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="F55" t="s">
+        <v>156</v>
+      </c>
+      <c r="H55" t="s">
+        <v>173</v>
+      </c>
+      <c r="J55" t="s">
+        <v>173</v>
+      </c>
+      <c r="L55" t="s">
+        <v>367</v>
+      </c>
+      <c r="N55" t="s">
+        <v>367</v>
+      </c>
+      <c r="R55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56" t="s">
+        <v>272</v>
+      </c>
+      <c r="D56" t="s">
+        <v>281</v>
+      </c>
+      <c r="F56" t="s">
+        <v>156</v>
+      </c>
+      <c r="H56" t="s">
+        <v>282</v>
+      </c>
+      <c r="J56" t="s">
+        <v>282</v>
+      </c>
+      <c r="L56" t="s">
+        <v>368</v>
+      </c>
+      <c r="N56" t="s">
+        <v>368</v>
+      </c>
+      <c r="R56" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" t="s">
+        <v>162</v>
+      </c>
+      <c r="H57" t="s">
+        <v>174</v>
+      </c>
+      <c r="J57" t="s">
+        <v>174</v>
+      </c>
+      <c r="L57" t="s">
+        <v>369</v>
+      </c>
+      <c r="N57" t="s">
+        <v>369</v>
+      </c>
+      <c r="R57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" t="s">
+        <v>274</v>
+      </c>
+      <c r="D58" t="s">
+        <v>284</v>
+      </c>
+      <c r="F58" t="s">
+        <v>285</v>
+      </c>
+      <c r="H58" t="s">
+        <v>286</v>
+      </c>
+      <c r="J58" t="s">
+        <v>286</v>
+      </c>
+      <c r="L58" t="s">
+        <v>370</v>
+      </c>
+      <c r="N58" t="s">
+        <v>370</v>
+      </c>
+      <c r="R58" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+      <c r="F59" t="s">
+        <v>142</v>
+      </c>
+      <c r="H59" t="s">
+        <v>175</v>
+      </c>
+      <c r="J59" t="s">
+        <v>175</v>
+      </c>
+      <c r="L59" t="s">
+        <v>371</v>
+      </c>
+      <c r="N59" t="s">
+        <v>371</v>
+      </c>
+      <c r="P59" t="s">
+        <v>191</v>
+      </c>
+      <c r="R59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>269</v>
+      </c>
+      <c r="B60" t="s">
+        <v>342</v>
+      </c>
+      <c r="D60" t="s">
+        <v>287</v>
+      </c>
+      <c r="F60" t="s">
+        <v>292</v>
+      </c>
+      <c r="H60" t="s">
+        <v>290</v>
+      </c>
+      <c r="J60" t="s">
+        <v>290</v>
+      </c>
+      <c r="L60" t="s">
+        <v>372</v>
+      </c>
+      <c r="N60" t="s">
+        <v>372</v>
+      </c>
+      <c r="P60" t="s">
+        <v>298</v>
+      </c>
+      <c r="R60" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" t="s">
+        <v>163</v>
+      </c>
+      <c r="H61" t="s">
+        <v>176</v>
+      </c>
+      <c r="J61" t="s">
+        <v>176</v>
+      </c>
+      <c r="L61" t="s">
+        <v>373</v>
+      </c>
+      <c r="N61" t="s">
+        <v>373</v>
+      </c>
+      <c r="R61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>270</v>
+      </c>
+      <c r="B62" t="s">
+        <v>248</v>
+      </c>
+      <c r="D62" t="s">
+        <v>288</v>
+      </c>
+      <c r="F62" t="s">
+        <v>293</v>
+      </c>
+      <c r="H62" t="s">
+        <v>291</v>
+      </c>
+      <c r="J62" t="s">
+        <v>291</v>
+      </c>
+      <c r="L62" t="s">
+        <v>374</v>
+      </c>
+      <c r="N62" t="s">
+        <v>374</v>
+      </c>
+      <c r="R62" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+      <c r="D63" t="s">
+        <v>109</v>
+      </c>
+      <c r="H63" t="s">
+        <v>172</v>
+      </c>
+      <c r="J63" t="s">
+        <v>172</v>
+      </c>
+      <c r="L63" t="s">
+        <v>375</v>
+      </c>
+      <c r="N63" t="s">
+        <v>375</v>
+      </c>
+      <c r="R63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>271</v>
+      </c>
+      <c r="B64" t="s">
+        <v>317</v>
+      </c>
+      <c r="D64" t="s">
+        <v>294</v>
+      </c>
+      <c r="H64" t="s">
+        <v>289</v>
+      </c>
+      <c r="J64" t="s">
+        <v>289</v>
+      </c>
+      <c r="L64" t="s">
+        <v>376</v>
+      </c>
+      <c r="N64" t="s">
+        <v>376</v>
+      </c>
+      <c r="R64" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" t="s">
+        <v>68</v>
+      </c>
+      <c r="R65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B67" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" t="s">
+        <v>208</v>
+      </c>
+      <c r="D68" t="s">
+        <v>206</v>
+      </c>
+      <c r="F68" t="s">
+        <v>208</v>
+      </c>
+      <c r="R68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" t="s">
+        <v>68</v>
+      </c>
+      <c r="H69" t="s">
+        <v>68</v>
+      </c>
+      <c r="J69" t="s">
+        <v>68</v>
+      </c>
+      <c r="L69" t="s">
+        <v>68</v>
+      </c>
+      <c r="N69" t="s">
+        <v>68</v>
+      </c>
+      <c r="R69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>299</v>
+      </c>
+      <c r="B70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" t="s">
+        <v>68</v>
+      </c>
+      <c r="H70" t="s">
+        <v>68</v>
+      </c>
+      <c r="J70" t="s">
+        <v>68</v>
+      </c>
+      <c r="L70" t="s">
+        <v>68</v>
+      </c>
+      <c r="N70" t="s">
+        <v>68</v>
+      </c>
+      <c r="R70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" t="s">
+        <v>68</v>
+      </c>
+      <c r="D71" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" t="s">
+        <v>68</v>
+      </c>
+      <c r="H71" t="s">
+        <v>68</v>
+      </c>
+      <c r="J71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L71" t="s">
+        <v>68</v>
+      </c>
+      <c r="N71" t="s">
+        <v>68</v>
+      </c>
+      <c r="R71" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>300</v>
+      </c>
+      <c r="B72" t="s">
+        <v>68</v>
+      </c>
+      <c r="D72" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" t="s">
+        <v>68</v>
+      </c>
+      <c r="H72" t="s">
+        <v>68</v>
+      </c>
+      <c r="J72" t="s">
+        <v>68</v>
+      </c>
+      <c r="L72" t="s">
+        <v>68</v>
+      </c>
+      <c r="N72" t="s">
+        <v>68</v>
+      </c>
+      <c r="R72" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" t="s">
+        <v>100</v>
+      </c>
+      <c r="F73" t="s">
+        <v>157</v>
+      </c>
+      <c r="R73" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>301</v>
+      </c>
+      <c r="B74" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" t="s">
+        <v>306</v>
+      </c>
+      <c r="F74" t="s">
+        <v>157</v>
+      </c>
+      <c r="R74" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>9</v>
+      </c>
+      <c r="B75" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" t="s">
+        <v>103</v>
+      </c>
+      <c r="F75" t="s">
+        <v>143</v>
+      </c>
+      <c r="R75" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>302</v>
+      </c>
+      <c r="B76" t="s">
+        <v>305</v>
+      </c>
+      <c r="D76" t="s">
+        <v>312</v>
+      </c>
+      <c r="F76" t="s">
+        <v>309</v>
+      </c>
+      <c r="R76" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" t="s">
+        <v>58</v>
+      </c>
+      <c r="D77" t="s">
+        <v>104</v>
+      </c>
+      <c r="F77" t="s">
+        <v>144</v>
+      </c>
+      <c r="P77" t="s">
+        <v>194</v>
+      </c>
+      <c r="R77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>303</v>
+      </c>
+      <c r="B78" t="s">
+        <v>249</v>
+      </c>
+      <c r="D78" t="s">
+        <v>313</v>
+      </c>
+      <c r="F78" t="s">
+        <v>310</v>
+      </c>
+      <c r="P78" t="s">
+        <v>308</v>
+      </c>
+      <c r="R78" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" t="s">
+        <v>105</v>
+      </c>
+      <c r="F79" t="s">
+        <v>145</v>
+      </c>
+      <c r="R79" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>304</v>
+      </c>
+      <c r="B80" t="s">
+        <v>328</v>
+      </c>
+      <c r="D80" t="s">
+        <v>314</v>
+      </c>
+      <c r="F80" t="s">
+        <v>311</v>
+      </c>
+      <c r="R80" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" t="s">
+        <v>120</v>
+      </c>
+      <c r="F81" t="s">
+        <v>159</v>
+      </c>
+      <c r="R81" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B82" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B83" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F85" t="s">
+        <v>37</v>
+      </c>
+      <c r="R85" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F86" t="s">
+        <v>326</v>
+      </c>
+      <c r="R86" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>27</v>
+      </c>
+      <c r="B87" t="s">
+        <v>37</v>
+      </c>
+      <c r="F87" t="s">
+        <v>37</v>
+      </c>
+      <c r="R87" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>318</v>
+      </c>
+      <c r="B88" t="s">
+        <v>326</v>
+      </c>
+      <c r="F88" t="s">
+        <v>326</v>
+      </c>
+      <c r="R88" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>62</v>
+      </c>
+      <c r="D89" t="s">
+        <v>92</v>
+      </c>
+      <c r="R89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>319</v>
+      </c>
+      <c r="B90" t="s">
+        <v>210</v>
+      </c>
+      <c r="D90" t="s">
+        <v>332</v>
+      </c>
+      <c r="R90" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" t="s">
+        <v>40</v>
+      </c>
+      <c r="D91" t="s">
+        <v>107</v>
+      </c>
+      <c r="F91" t="s">
+        <v>158</v>
+      </c>
+      <c r="R91" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>320</v>
+      </c>
+      <c r="B92" t="s">
+        <v>327</v>
+      </c>
+      <c r="D92" t="s">
+        <v>333</v>
+      </c>
+      <c r="F92" t="s">
+        <v>158</v>
+      </c>
+      <c r="R92" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" t="s">
+        <v>51</v>
+      </c>
+      <c r="D93" t="s">
+        <v>106</v>
+      </c>
+      <c r="F93" t="s">
+        <v>161</v>
+      </c>
+      <c r="R93" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>321</v>
+      </c>
+      <c r="B94" t="s">
+        <v>329</v>
+      </c>
+      <c r="D94" t="s">
+        <v>334</v>
+      </c>
+      <c r="F94" t="s">
+        <v>161</v>
+      </c>
+      <c r="R94" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" t="s">
+        <v>61</v>
+      </c>
+      <c r="D95" t="s">
+        <v>123</v>
+      </c>
+      <c r="P95" t="s">
+        <v>195</v>
+      </c>
+      <c r="R95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>322</v>
+      </c>
+      <c r="B96" t="s">
+        <v>246</v>
+      </c>
+      <c r="D96" t="s">
+        <v>335</v>
+      </c>
+      <c r="P96" t="s">
+        <v>338</v>
+      </c>
+      <c r="R96" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B97" t="s">
+        <v>60</v>
+      </c>
+      <c r="D97" t="s">
+        <v>121</v>
+      </c>
+      <c r="F97" t="s">
+        <v>164</v>
+      </c>
+      <c r="R97" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>323</v>
+      </c>
+      <c r="B98" t="s">
+        <v>278</v>
+      </c>
+      <c r="D98" t="s">
+        <v>336</v>
+      </c>
+      <c r="F98" t="s">
+        <v>164</v>
+      </c>
+      <c r="R98" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" t="s">
+        <v>64</v>
+      </c>
+      <c r="D99" t="s">
+        <v>122</v>
+      </c>
+      <c r="F99" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>324</v>
+      </c>
+      <c r="B100" t="s">
+        <v>276</v>
+      </c>
+      <c r="D100" t="s">
+        <v>337</v>
+      </c>
+      <c r="F100" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" t="s">
+        <v>36</v>
+      </c>
+      <c r="F127" t="s">
+        <v>36</v>
+      </c>
+      <c r="H127" t="s">
+        <v>36</v>
+      </c>
+      <c r="J127" t="s">
+        <v>36</v>
+      </c>
+      <c r="L127" t="s">
+        <v>36</v>
+      </c>
+      <c r="N127" t="s">
+        <v>36</v>
+      </c>
+      <c r="T127">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>339</v>
+      </c>
+      <c r="B128" t="s">
+        <v>340</v>
+      </c>
+      <c r="F128" t="s">
+        <v>340</v>
+      </c>
+      <c r="H128" t="s">
+        <v>340</v>
+      </c>
+      <c r="J128" t="s">
+        <v>340</v>
+      </c>
+      <c r="L128" t="s">
+        <v>340</v>
+      </c>
+      <c r="N128" t="s">
+        <v>340</v>
+      </c>
+      <c r="T128">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D23" r:id="rId1"/>
+    <hyperlink ref="D26" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T122"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D58" sqref="D58:R58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" t="s">
+        <v>238</v>
+      </c>
+      <c r="R3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>55</v>
       </c>
       <c r="D4" t="s">
@@ -2621,6 +4661,24 @@
       <c r="B57" t="s">
         <v>202</v>
       </c>
+      <c r="D57" t="s">
+        <v>294</v>
+      </c>
+      <c r="H57" t="s">
+        <v>289</v>
+      </c>
+      <c r="J57" t="s">
+        <v>289</v>
+      </c>
+      <c r="L57" t="s">
+        <v>376</v>
+      </c>
+      <c r="N57" t="s">
+        <v>376</v>
+      </c>
+      <c r="R57" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -2628,6 +4686,24 @@
       </c>
       <c r="B58" t="s">
         <v>204</v>
+      </c>
+      <c r="D58" t="s">
+        <v>294</v>
+      </c>
+      <c r="H58" t="s">
+        <v>289</v>
+      </c>
+      <c r="J58" t="s">
+        <v>289</v>
+      </c>
+      <c r="L58" t="s">
+        <v>376</v>
+      </c>
+      <c r="N58" t="s">
+        <v>376</v>
+      </c>
+      <c r="R58" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -3422,7 +5498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T120"/>
   <sheetViews>
@@ -5233,7 +7309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add changes to support aliases for layers - ie., different key combinations for same layer
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Keys.DVORAK" sheetId="6" r:id="rId1"/>
     <sheet name="Keys.Colemak" sheetId="5" r:id="rId2"/>
     <sheet name="Keys.QWERTY" sheetId="4" r:id="rId3"/>
     <sheet name="Layers" sheetId="3" r:id="rId4"/>
+    <sheet name="Layer Aliases" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="399">
   <si>
     <t>a</t>
   </si>
@@ -1221,6 +1222,21 @@
   </si>
   <si>
     <t>+{j}</t>
+  </si>
+  <si>
+    <t>{Blind}{)}</t>
+  </si>
+  <si>
+    <t>+Space</t>
+  </si>
+  <si>
+    <t>+*Space</t>
+  </si>
+  <si>
+    <t>ShiftGreen</t>
+  </si>
+  <si>
+    <t>LayerAlias</t>
   </si>
 </sst>
 </file>
@@ -1265,12 +1281,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1305,7 +1324,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HotKeys.DVORAK" displayName="HotKeys.DVORAK" ref="A1:T128" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HotKeys.DVORAK" displayName="HotKeys.DVORAK" ref="A1:T128" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:T128"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
@@ -1334,7 +1353,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T122" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T122" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:T122"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
@@ -1363,8 +1382,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:T120" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:T120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:T122" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:T122"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
@@ -1392,12 +1411,23 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Layer"/>
-    <tableColumn id="2" name="Keys" dataDxfId="1"/>
+    <tableColumn id="2" name="Keys" dataDxfId="0"/>
     <tableColumn id="3" name="Delay"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="LayerAliases" displayName="LayerAliases" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="LayerAlias"/>
+    <tableColumn id="2" name="Layer"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1668,11 +1698,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B110" sqref="B110"/>
+      <selection pane="bottomRight" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5500,13 +5530,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T120"/>
+  <dimension ref="A1:T122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="N120" sqref="N120:N121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6833,7 +6863,7 @@
         <v>69</v>
       </c>
       <c r="D73" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F73" t="s">
         <v>159</v>
@@ -6849,6 +6879,9 @@
       <c r="B74" t="s">
         <v>134</v>
       </c>
+      <c r="D74" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
@@ -6857,6 +6890,9 @@
       <c r="B75" t="s">
         <v>202</v>
       </c>
+      <c r="D75" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -6865,6 +6901,9 @@
       <c r="B76" t="s">
         <v>204</v>
       </c>
+      <c r="D76" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -7026,7 +7065,7 @@
         <v>65</v>
       </c>
       <c r="D87" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="P87" t="s">
         <v>195</v>
@@ -7043,7 +7082,7 @@
         <v>330</v>
       </c>
       <c r="D88" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="P88" t="s">
         <v>338</v>
@@ -7060,7 +7099,7 @@
         <v>66</v>
       </c>
       <c r="D89" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F89" t="s">
         <v>164</v>
@@ -7077,7 +7116,7 @@
         <v>307</v>
       </c>
       <c r="D90" t="s">
-        <v>336</v>
+        <v>394</v>
       </c>
       <c r="F90" t="s">
         <v>164</v>
@@ -7271,8 +7310,8 @@
       </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>339</v>
+      <c r="A120" s="1" t="s">
+        <v>395</v>
       </c>
       <c r="B120" t="s">
         <v>340</v>
@@ -7292,7 +7331,53 @@
       <c r="N120" t="s">
         <v>340</v>
       </c>
-      <c r="T120">
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B121" t="s">
+        <v>340</v>
+      </c>
+      <c r="F121" t="s">
+        <v>340</v>
+      </c>
+      <c r="H121" t="s">
+        <v>340</v>
+      </c>
+      <c r="J121" t="s">
+        <v>340</v>
+      </c>
+      <c r="L121" t="s">
+        <v>340</v>
+      </c>
+      <c r="N121" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>339</v>
+      </c>
+      <c r="B122" t="s">
+        <v>340</v>
+      </c>
+      <c r="F122" t="s">
+        <v>340</v>
+      </c>
+      <c r="H122" t="s">
+        <v>340</v>
+      </c>
+      <c r="J122" t="s">
+        <v>340</v>
+      </c>
+      <c r="L122" t="s">
+        <v>340</v>
+      </c>
+      <c r="N122" t="s">
+        <v>340</v>
+      </c>
+      <c r="T122">
         <v>100</v>
       </c>
     </row>
@@ -7311,10 +7396,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7405,10 +7490,68 @@
         <v>351</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>397</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove the Function(Low/High)Right columns and use layer alias instead.  One layer definition; multiple aliases (key combinations) for that layer.
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Keys.DVORAK" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="395">
   <si>
     <t>a</t>
   </si>
@@ -1081,12 +1081,6 @@
     <t>*x</t>
   </si>
   <si>
-    <t>FunctionLowRight Down</t>
-  </si>
-  <si>
-    <t>FunctionLowRight Up</t>
-  </si>
-  <si>
     <t>FunctionLowRight</t>
   </si>
   <si>
@@ -1105,12 +1099,6 @@
   </si>
   <si>
     <t>FunctionHigh Up</t>
-  </si>
-  <si>
-    <t>FunctionHighRight Down</t>
-  </si>
-  <si>
-    <t>FunctionHighRight Up</t>
   </si>
   <si>
     <t>{F11}</t>
@@ -1324,9 +1312,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HotKeys.DVORAK" displayName="HotKeys.DVORAK" ref="A1:T128" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:T128"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HotKeys.DVORAK" displayName="HotKeys.DVORAK" ref="A1:P128" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:P128"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
     <tableColumn id="3" name="Alpha Up"/>
@@ -1336,12 +1324,8 @@
     <tableColumn id="7" name="Edit Up"/>
     <tableColumn id="8" name="FunctionLow Down"/>
     <tableColumn id="9" name="FunctionLow Up"/>
-    <tableColumn id="15" name="FunctionLowRight Down"/>
-    <tableColumn id="16" name="FunctionLowRight Up"/>
     <tableColumn id="20" name="FunctionHigh Down"/>
     <tableColumn id="19" name="FunctionHigh Up"/>
-    <tableColumn id="18" name="FunctionHighRight Down"/>
-    <tableColumn id="17" name="FunctionHighRight Up"/>
     <tableColumn id="11" name="Media Down"/>
     <tableColumn id="12" name="Media Up"/>
     <tableColumn id="10" name="Green Media Down"/>
@@ -1353,9 +1337,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:T122" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:T122"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="HotKeys.Colemak" displayName="HotKeys.Colemak" ref="A1:P122" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:P122"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
     <tableColumn id="3" name="Alpha Up"/>
@@ -1365,12 +1349,8 @@
     <tableColumn id="7" name="Edit Up"/>
     <tableColumn id="8" name="FunctionLow Down"/>
     <tableColumn id="9" name="FunctionLow Up"/>
-    <tableColumn id="15" name="FunctionLowRight Down"/>
-    <tableColumn id="16" name="FunctionLowRight Up"/>
     <tableColumn id="20" name="FunctionHigh Down"/>
     <tableColumn id="19" name="FunctionHigh Up"/>
-    <tableColumn id="18" name="FunctionHighRight Down"/>
-    <tableColumn id="17" name="FunctionHighRight Up"/>
     <tableColumn id="11" name="Media Down"/>
     <tableColumn id="12" name="Media Up"/>
     <tableColumn id="10" name="Green Media Down"/>
@@ -1382,9 +1362,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:T122" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:T122"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:P122" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:P122"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
     <tableColumn id="3" name="Alpha Up"/>
@@ -1394,12 +1374,8 @@
     <tableColumn id="7" name="Edit Up"/>
     <tableColumn id="8" name="FunctionLow Down"/>
     <tableColumn id="9" name="FunctionLow Up"/>
-    <tableColumn id="15" name="FunctionLowRight Down"/>
-    <tableColumn id="16" name="FunctionLowRight Up"/>
     <tableColumn id="20" name="FunctionHigh Down"/>
     <tableColumn id="19" name="FunctionHigh Up"/>
-    <tableColumn id="18" name="FunctionHighRight Down"/>
-    <tableColumn id="17" name="FunctionHighRight Up"/>
     <tableColumn id="11" name="Media Down"/>
     <tableColumn id="12" name="Media Up"/>
     <tableColumn id="10" name="Green Media Down"/>
@@ -1423,8 +1399,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="LayerAliases" displayName="LayerAliases" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="LayerAliases" displayName="LayerAliases" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="LayerAlias"/>
     <tableColumn id="2" name="Layer"/>
@@ -1696,13 +1672,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T128"/>
+  <dimension ref="A1:P128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D81" sqref="D81"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,17 +1691,15 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
@@ -1754,40 +1728,28 @@
         <v>166</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>353</v>
+        <v>192</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>354</v>
+        <v>193</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>355</v>
+        <v>200</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>356</v>
+        <v>199</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="T1" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1800,11 +1762,11 @@
       <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="R2" t="s">
+      <c r="N2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -1817,11 +1779,11 @@
       <c r="F3" t="s">
         <v>238</v>
       </c>
-      <c r="R3" t="s">
+      <c r="N3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1835,18 +1797,12 @@
         <v>167</v>
       </c>
       <c r="J4" t="s">
-        <v>167</v>
-      </c>
-      <c r="L4" t="s">
-        <v>357</v>
-      </c>
-      <c r="N4" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s">
         <v>204</v>
@@ -1858,18 +1814,12 @@
         <v>255</v>
       </c>
       <c r="J5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L5" t="s">
-        <v>358</v>
-      </c>
-      <c r="N5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B6" t="s">
         <v>204</v>
@@ -1881,16 +1831,10 @@
         <v>255</v>
       </c>
       <c r="J6" t="s">
-        <v>255</v>
-      </c>
-      <c r="L6" t="s">
-        <v>358</v>
-      </c>
-      <c r="N6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>240</v>
       </c>
@@ -1904,16 +1848,10 @@
         <v>255</v>
       </c>
       <c r="J7" t="s">
-        <v>255</v>
-      </c>
-      <c r="L7" t="s">
-        <v>358</v>
-      </c>
-      <c r="N7" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1927,18 +1865,12 @@
         <v>168</v>
       </c>
       <c r="J8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L8" t="s">
-        <v>359</v>
-      </c>
-      <c r="N8" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B9" t="s">
         <v>330</v>
@@ -1950,18 +1882,12 @@
         <v>256</v>
       </c>
       <c r="J9" t="s">
-        <v>256</v>
-      </c>
-      <c r="L9" t="s">
-        <v>360</v>
-      </c>
-      <c r="N9" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B10" t="s">
         <v>330</v>
@@ -1973,16 +1899,10 @@
         <v>256</v>
       </c>
       <c r="J10" t="s">
-        <v>256</v>
-      </c>
-      <c r="L10" t="s">
-        <v>360</v>
-      </c>
-      <c r="N10" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>241</v>
       </c>
@@ -1996,16 +1916,10 @@
         <v>256</v>
       </c>
       <c r="J11" t="s">
-        <v>256</v>
-      </c>
-      <c r="L11" t="s">
-        <v>360</v>
-      </c>
-      <c r="N11" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2019,18 +1933,12 @@
         <v>169</v>
       </c>
       <c r="J12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L12" t="s">
-        <v>361</v>
-      </c>
-      <c r="N12" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B13" t="s">
         <v>307</v>
@@ -2042,18 +1950,12 @@
         <v>257</v>
       </c>
       <c r="J13" t="s">
-        <v>257</v>
-      </c>
-      <c r="L13" t="s">
-        <v>362</v>
-      </c>
-      <c r="N13" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B14" t="s">
         <v>307</v>
@@ -2065,16 +1967,10 @@
         <v>257</v>
       </c>
       <c r="J14" t="s">
-        <v>257</v>
-      </c>
-      <c r="L14" t="s">
-        <v>362</v>
-      </c>
-      <c r="N14" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -2088,16 +1984,10 @@
         <v>257</v>
       </c>
       <c r="J15" t="s">
-        <v>257</v>
-      </c>
-      <c r="L15" t="s">
-        <v>362</v>
-      </c>
-      <c r="N15" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2111,16 +2001,10 @@
         <v>170</v>
       </c>
       <c r="J16" t="s">
-        <v>170</v>
-      </c>
-      <c r="L16" t="s">
-        <v>363</v>
-      </c>
-      <c r="N16" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>243</v>
       </c>
@@ -2134,16 +2018,10 @@
         <v>258</v>
       </c>
       <c r="J17" t="s">
-        <v>258</v>
-      </c>
-      <c r="L17" t="s">
-        <v>364</v>
-      </c>
-      <c r="N17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2157,16 +2035,10 @@
         <v>171</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
-      </c>
-      <c r="L18" t="s">
-        <v>365</v>
-      </c>
-      <c r="N18" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>244</v>
       </c>
@@ -2180,16 +2052,10 @@
         <v>259</v>
       </c>
       <c r="J19" t="s">
-        <v>259</v>
-      </c>
-      <c r="L19" t="s">
-        <v>366</v>
-      </c>
-      <c r="N19" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -2197,7 +2063,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2208,7 +2074,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>260</v>
       </c>
@@ -2219,7 +2085,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2236,18 +2102,18 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>213</v>
       </c>
@@ -2258,7 +2124,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>216</v>
       </c>
@@ -2275,7 +2141,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2286,18 +2152,18 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D28" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>223</v>
       </c>
@@ -2308,7 +2174,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>224</v>
       </c>
@@ -2319,7 +2185,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>225</v>
       </c>
@@ -2330,7 +2196,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>226</v>
       </c>
@@ -2442,7 +2308,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B42" t="s">
         <v>335</v>
@@ -2453,7 +2319,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B43" t="s">
         <v>335</v>
@@ -2489,7 +2355,7 @@
         <v>130</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D46" t="s">
         <v>132</v>
@@ -2517,7 +2383,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2528,18 +2394,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D50" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>341</v>
       </c>
@@ -2550,7 +2416,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>344</v>
       </c>
@@ -2561,7 +2427,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -2572,7 +2438,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>266</v>
       </c>
@@ -2583,7 +2449,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>23</v>
       </c>
@@ -2600,19 +2466,13 @@
         <v>173</v>
       </c>
       <c r="J55" t="s">
-        <v>173</v>
-      </c>
-      <c r="L55" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="N55" t="s">
-        <v>367</v>
-      </c>
-      <c r="R55" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>267</v>
       </c>
@@ -2629,19 +2489,13 @@
         <v>282</v>
       </c>
       <c r="J56" t="s">
-        <v>282</v>
-      </c>
-      <c r="L56" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="N56" t="s">
-        <v>368</v>
-      </c>
-      <c r="R56" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2658,19 +2512,13 @@
         <v>174</v>
       </c>
       <c r="J57" t="s">
-        <v>174</v>
-      </c>
-      <c r="L57" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="N57" t="s">
-        <v>369</v>
-      </c>
-      <c r="R57" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>268</v>
       </c>
@@ -2687,19 +2535,13 @@
         <v>286</v>
       </c>
       <c r="J58" t="s">
-        <v>286</v>
-      </c>
-      <c r="L58" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="N58" t="s">
-        <v>370</v>
-      </c>
-      <c r="R58" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2716,22 +2558,16 @@
         <v>175</v>
       </c>
       <c r="J59" t="s">
-        <v>175</v>
+        <v>367</v>
       </c>
       <c r="L59" t="s">
-        <v>371</v>
+        <v>191</v>
       </c>
       <c r="N59" t="s">
-        <v>371</v>
-      </c>
-      <c r="P59" t="s">
-        <v>191</v>
-      </c>
-      <c r="R59" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>269</v>
       </c>
@@ -2748,22 +2584,16 @@
         <v>290</v>
       </c>
       <c r="J60" t="s">
-        <v>290</v>
+        <v>368</v>
       </c>
       <c r="L60" t="s">
-        <v>372</v>
+        <v>298</v>
       </c>
       <c r="N60" t="s">
-        <v>372</v>
-      </c>
-      <c r="P60" t="s">
-        <v>298</v>
-      </c>
-      <c r="R60" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -2780,19 +2610,13 @@
         <v>176</v>
       </c>
       <c r="J61" t="s">
-        <v>176</v>
-      </c>
-      <c r="L61" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="N61" t="s">
-        <v>373</v>
-      </c>
-      <c r="R61" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>270</v>
       </c>
@@ -2809,19 +2633,13 @@
         <v>291</v>
       </c>
       <c r="J62" t="s">
-        <v>291</v>
-      </c>
-      <c r="L62" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="N62" t="s">
-        <v>374</v>
-      </c>
-      <c r="R62" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -2835,19 +2653,13 @@
         <v>172</v>
       </c>
       <c r="J63" t="s">
-        <v>172</v>
-      </c>
-      <c r="L63" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="N63" t="s">
-        <v>375</v>
-      </c>
-      <c r="R63" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>271</v>
       </c>
@@ -2861,19 +2673,13 @@
         <v>289</v>
       </c>
       <c r="J64" t="s">
-        <v>289</v>
-      </c>
-      <c r="L64" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N64" t="s">
-        <v>376</v>
-      </c>
-      <c r="R64" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>31</v>
       </c>
@@ -2886,11 +2692,11 @@
       <c r="F65" t="s">
         <v>68</v>
       </c>
-      <c r="R65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -2898,7 +2704,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>205</v>
       </c>
@@ -2906,7 +2712,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>207</v>
       </c>
@@ -2919,11 +2725,11 @@
       <c r="F68" t="s">
         <v>208</v>
       </c>
-      <c r="R68" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>32</v>
       </c>
@@ -2942,17 +2748,11 @@
       <c r="J69" t="s">
         <v>68</v>
       </c>
-      <c r="L69" t="s">
-        <v>68</v>
-      </c>
       <c r="N69" t="s">
         <v>68</v>
       </c>
-      <c r="R69" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>299</v>
       </c>
@@ -2971,17 +2771,11 @@
       <c r="J70" t="s">
         <v>68</v>
       </c>
-      <c r="L70" t="s">
-        <v>68</v>
-      </c>
       <c r="N70" t="s">
         <v>68</v>
       </c>
-      <c r="R70" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>33</v>
       </c>
@@ -3000,17 +2794,11 @@
       <c r="J71" t="s">
         <v>68</v>
       </c>
-      <c r="L71" t="s">
-        <v>68</v>
-      </c>
       <c r="N71" t="s">
         <v>68</v>
       </c>
-      <c r="R71" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>300</v>
       </c>
@@ -3029,17 +2817,11 @@
       <c r="J72" t="s">
         <v>68</v>
       </c>
-      <c r="L72" t="s">
-        <v>68</v>
-      </c>
       <c r="N72" t="s">
         <v>68</v>
       </c>
-      <c r="R72" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -3052,11 +2834,11 @@
       <c r="F73" t="s">
         <v>157</v>
       </c>
-      <c r="R73" t="s">
+      <c r="N73" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>301</v>
       </c>
@@ -3069,11 +2851,11 @@
       <c r="F74" t="s">
         <v>157</v>
       </c>
-      <c r="R74" t="s">
+      <c r="N74" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -3086,11 +2868,11 @@
       <c r="F75" t="s">
         <v>143</v>
       </c>
-      <c r="R75" t="s">
+      <c r="N75" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>302</v>
       </c>
@@ -3103,11 +2885,11 @@
       <c r="F76" t="s">
         <v>309</v>
       </c>
-      <c r="R76" t="s">
+      <c r="N76" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>25</v>
       </c>
@@ -3120,14 +2902,14 @@
       <c r="F77" t="s">
         <v>144</v>
       </c>
-      <c r="P77" t="s">
+      <c r="L77" t="s">
         <v>194</v>
       </c>
-      <c r="R77" t="s">
+      <c r="N77" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>303</v>
       </c>
@@ -3140,14 +2922,14 @@
       <c r="F78" t="s">
         <v>310</v>
       </c>
-      <c r="P78" t="s">
+      <c r="L78" t="s">
         <v>308</v>
       </c>
-      <c r="R78" t="s">
+      <c r="N78" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -3160,11 +2942,11 @@
       <c r="F79" t="s">
         <v>145</v>
       </c>
-      <c r="R79" t="s">
+      <c r="N79" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>304</v>
       </c>
@@ -3177,11 +2959,11 @@
       <c r="F80" t="s">
         <v>311</v>
       </c>
-      <c r="R80" t="s">
+      <c r="N80" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>34</v>
       </c>
@@ -3194,11 +2976,11 @@
       <c r="F81" t="s">
         <v>159</v>
       </c>
-      <c r="R81" t="s">
+      <c r="N81" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>133</v>
       </c>
@@ -3206,7 +2988,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>201</v>
       </c>
@@ -3214,7 +2996,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>203</v>
       </c>
@@ -3222,7 +3004,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>35</v>
       </c>
@@ -3232,11 +3014,11 @@
       <c r="F85" t="s">
         <v>37</v>
       </c>
-      <c r="R85" t="s">
+      <c r="N85" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>325</v>
       </c>
@@ -3246,11 +3028,11 @@
       <c r="F86" t="s">
         <v>326</v>
       </c>
-      <c r="R86" t="s">
+      <c r="N86" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>27</v>
       </c>
@@ -3260,11 +3042,11 @@
       <c r="F87" t="s">
         <v>37</v>
       </c>
-      <c r="R87" t="s">
+      <c r="N87" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>318</v>
       </c>
@@ -3274,11 +3056,11 @@
       <c r="F88" t="s">
         <v>326</v>
       </c>
-      <c r="R88" t="s">
+      <c r="N88" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -3288,11 +3070,11 @@
       <c r="D89" t="s">
         <v>92</v>
       </c>
-      <c r="R89" t="s">
+      <c r="N89" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>319</v>
       </c>
@@ -3302,11 +3084,11 @@
       <c r="D90" t="s">
         <v>332</v>
       </c>
-      <c r="R90" t="s">
+      <c r="N90" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -3319,11 +3101,11 @@
       <c r="F91" t="s">
         <v>158</v>
       </c>
-      <c r="R91" t="s">
+      <c r="N91" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>320</v>
       </c>
@@ -3336,11 +3118,11 @@
       <c r="F92" t="s">
         <v>158</v>
       </c>
-      <c r="R92" t="s">
+      <c r="N92" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -3353,11 +3135,11 @@
       <c r="F93" t="s">
         <v>161</v>
       </c>
-      <c r="R93" t="s">
+      <c r="N93" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>321</v>
       </c>
@@ -3370,11 +3152,11 @@
       <c r="F94" t="s">
         <v>161</v>
       </c>
-      <c r="R94" t="s">
+      <c r="N94" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -3384,14 +3166,14 @@
       <c r="D95" t="s">
         <v>123</v>
       </c>
-      <c r="P95" t="s">
+      <c r="L95" t="s">
         <v>195</v>
       </c>
-      <c r="R95" t="s">
+      <c r="N95" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>322</v>
       </c>
@@ -3401,14 +3183,14 @@
       <c r="D96" t="s">
         <v>335</v>
       </c>
-      <c r="P96" t="s">
+      <c r="L96" t="s">
         <v>338</v>
       </c>
-      <c r="R96" t="s">
+      <c r="N96" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>29</v>
       </c>
@@ -3421,11 +3203,11 @@
       <c r="F97" t="s">
         <v>164</v>
       </c>
-      <c r="R97" t="s">
+      <c r="N97" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>323</v>
       </c>
@@ -3438,11 +3220,11 @@
       <c r="F98" t="s">
         <v>164</v>
       </c>
-      <c r="R98" t="s">
+      <c r="N98" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>30</v>
       </c>
@@ -3456,7 +3238,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>324</v>
       </c>
@@ -3470,137 +3252,137 @@
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -3616,17 +3398,11 @@
       <c r="J127" t="s">
         <v>36</v>
       </c>
-      <c r="L127" t="s">
-        <v>36</v>
-      </c>
-      <c r="N127" t="s">
-        <v>36</v>
-      </c>
-      <c r="T127">
+      <c r="P127">
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>339</v>
       </c>
@@ -3642,13 +3418,7 @@
       <c r="J128" t="s">
         <v>340</v>
       </c>
-      <c r="L128" t="s">
-        <v>340</v>
-      </c>
-      <c r="N128" t="s">
-        <v>340</v>
-      </c>
-      <c r="T128">
+      <c r="P128">
         <v>100</v>
       </c>
     </row>
@@ -3667,13 +3437,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T122"/>
+  <dimension ref="A1:P122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D58" sqref="D58:R58"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3686,17 +3456,15 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
@@ -3725,40 +3493,28 @@
         <v>166</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>353</v>
+        <v>192</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>354</v>
+        <v>193</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>355</v>
+        <v>200</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>356</v>
+        <v>199</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="T1" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -3771,11 +3527,11 @@
       <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="R2" t="s">
+      <c r="N2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -3788,11 +3544,11 @@
       <c r="F3" t="s">
         <v>238</v>
       </c>
-      <c r="R3" t="s">
+      <c r="N3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3806,16 +3562,10 @@
         <v>167</v>
       </c>
       <c r="J4" t="s">
-        <v>167</v>
-      </c>
-      <c r="L4" t="s">
-        <v>357</v>
-      </c>
-      <c r="N4" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -3829,16 +3579,10 @@
         <v>255</v>
       </c>
       <c r="J5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L5" t="s">
-        <v>358</v>
-      </c>
-      <c r="N5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3852,16 +3596,10 @@
         <v>168</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
-      </c>
-      <c r="L6" t="s">
-        <v>359</v>
-      </c>
-      <c r="N6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
@@ -3875,16 +3613,10 @@
         <v>256</v>
       </c>
       <c r="J7" t="s">
-        <v>256</v>
-      </c>
-      <c r="L7" t="s">
-        <v>360</v>
-      </c>
-      <c r="N7" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3898,16 +3630,10 @@
         <v>169</v>
       </c>
       <c r="J8" t="s">
-        <v>169</v>
-      </c>
-      <c r="L8" t="s">
-        <v>361</v>
-      </c>
-      <c r="N8" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -3921,16 +3647,10 @@
         <v>257</v>
       </c>
       <c r="J9" t="s">
-        <v>257</v>
-      </c>
-      <c r="L9" t="s">
-        <v>362</v>
-      </c>
-      <c r="N9" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3944,16 +3664,10 @@
         <v>170</v>
       </c>
       <c r="J10" t="s">
-        <v>170</v>
-      </c>
-      <c r="L10" t="s">
-        <v>363</v>
-      </c>
-      <c r="N10" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -3967,16 +3681,10 @@
         <v>258</v>
       </c>
       <c r="J11" t="s">
-        <v>258</v>
-      </c>
-      <c r="L11" t="s">
-        <v>364</v>
-      </c>
-      <c r="N11" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3990,16 +3698,10 @@
         <v>171</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
-      </c>
-      <c r="L12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N12" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>244</v>
       </c>
@@ -4013,16 +3715,10 @@
         <v>259</v>
       </c>
       <c r="J13" t="s">
-        <v>259</v>
-      </c>
-      <c r="L13" t="s">
-        <v>366</v>
-      </c>
-      <c r="N13" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -4030,7 +3726,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4041,7 +3737,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>260</v>
       </c>
@@ -4074,7 +3770,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>128</v>
@@ -4240,7 +3936,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -4251,7 +3947,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>264</v>
       </c>
@@ -4262,7 +3958,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -4273,7 +3969,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>265</v>
       </c>
@@ -4284,7 +3980,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -4295,7 +3991,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>130</v>
       </c>
@@ -4306,7 +4002,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>209</v>
       </c>
@@ -4317,7 +4013,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>346</v>
       </c>
@@ -4328,7 +4024,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -4339,7 +4035,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -4350,7 +4046,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>341</v>
       </c>
@@ -4361,7 +4057,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>344</v>
       </c>
@@ -4372,7 +4068,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -4383,7 +4079,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>266</v>
       </c>
@@ -4394,7 +4090,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -4411,19 +4107,13 @@
         <v>173</v>
       </c>
       <c r="J47" t="s">
-        <v>173</v>
-      </c>
-      <c r="L47" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="N47" t="s">
-        <v>367</v>
-      </c>
-      <c r="R47" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>267</v>
       </c>
@@ -4440,19 +4130,13 @@
         <v>282</v>
       </c>
       <c r="J48" t="s">
-        <v>282</v>
-      </c>
-      <c r="L48" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="N48" t="s">
-        <v>368</v>
-      </c>
-      <c r="R48" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -4469,19 +4153,13 @@
         <v>174</v>
       </c>
       <c r="J49" t="s">
-        <v>174</v>
-      </c>
-      <c r="L49" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="N49" t="s">
-        <v>369</v>
-      </c>
-      <c r="R49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>268</v>
       </c>
@@ -4498,19 +4176,13 @@
         <v>286</v>
       </c>
       <c r="J50" t="s">
-        <v>286</v>
-      </c>
-      <c r="L50" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="N50" t="s">
-        <v>370</v>
-      </c>
-      <c r="R50" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -4527,22 +4199,16 @@
         <v>175</v>
       </c>
       <c r="J51" t="s">
-        <v>175</v>
+        <v>367</v>
       </c>
       <c r="L51" t="s">
-        <v>371</v>
+        <v>191</v>
       </c>
       <c r="N51" t="s">
-        <v>371</v>
-      </c>
-      <c r="P51" t="s">
-        <v>191</v>
-      </c>
-      <c r="R51" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>269</v>
       </c>
@@ -4559,22 +4225,16 @@
         <v>290</v>
       </c>
       <c r="J52" t="s">
-        <v>290</v>
+        <v>368</v>
       </c>
       <c r="L52" t="s">
-        <v>372</v>
+        <v>298</v>
       </c>
       <c r="N52" t="s">
-        <v>372</v>
-      </c>
-      <c r="P52" t="s">
-        <v>298</v>
-      </c>
-      <c r="R52" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -4591,19 +4251,13 @@
         <v>176</v>
       </c>
       <c r="J53" t="s">
-        <v>176</v>
-      </c>
-      <c r="L53" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="N53" t="s">
-        <v>373</v>
-      </c>
-      <c r="R53" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>270</v>
       </c>
@@ -4620,19 +4274,13 @@
         <v>291</v>
       </c>
       <c r="J54" t="s">
-        <v>291</v>
-      </c>
-      <c r="L54" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="N54" t="s">
-        <v>374</v>
-      </c>
-      <c r="R54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -4646,21 +4294,15 @@
         <v>172</v>
       </c>
       <c r="J55" t="s">
-        <v>172</v>
-      </c>
-      <c r="L55" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="N55" t="s">
-        <v>375</v>
-      </c>
-      <c r="R55" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B56" t="s">
         <v>134</v>
@@ -4672,21 +4314,15 @@
         <v>289</v>
       </c>
       <c r="J56" t="s">
-        <v>289</v>
-      </c>
-      <c r="L56" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N56" t="s">
-        <v>376</v>
-      </c>
-      <c r="R56" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B57" t="s">
         <v>202</v>
@@ -4698,19 +4334,13 @@
         <v>289</v>
       </c>
       <c r="J57" t="s">
-        <v>289</v>
-      </c>
-      <c r="L57" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N57" t="s">
-        <v>376</v>
-      </c>
-      <c r="R57" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>271</v>
       </c>
@@ -4724,19 +4354,13 @@
         <v>289</v>
       </c>
       <c r="J58" t="s">
-        <v>289</v>
-      </c>
-      <c r="L58" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N58" t="s">
-        <v>376</v>
-      </c>
-      <c r="R58" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -4749,11 +4373,11 @@
       <c r="F59" t="s">
         <v>68</v>
       </c>
-      <c r="R59" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
@@ -4761,7 +4385,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>205</v>
       </c>
@@ -4769,7 +4393,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>207</v>
       </c>
@@ -4782,11 +4406,11 @@
       <c r="F62" t="s">
         <v>208</v>
       </c>
-      <c r="R62" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>32</v>
       </c>
@@ -4805,17 +4429,11 @@
       <c r="J63" t="s">
         <v>68</v>
       </c>
-      <c r="L63" t="s">
-        <v>68</v>
-      </c>
       <c r="N63" t="s">
         <v>68</v>
       </c>
-      <c r="R63" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>299</v>
       </c>
@@ -4834,17 +4452,11 @@
       <c r="J64" t="s">
         <v>68</v>
       </c>
-      <c r="L64" t="s">
-        <v>68</v>
-      </c>
       <c r="N64" t="s">
         <v>68</v>
       </c>
-      <c r="R64" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>33</v>
       </c>
@@ -4863,17 +4475,11 @@
       <c r="J65" t="s">
         <v>68</v>
       </c>
-      <c r="L65" t="s">
-        <v>68</v>
-      </c>
       <c r="N65" t="s">
         <v>68</v>
       </c>
-      <c r="R65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>300</v>
       </c>
@@ -4892,17 +4498,11 @@
       <c r="J66" t="s">
         <v>68</v>
       </c>
-      <c r="L66" t="s">
-        <v>68</v>
-      </c>
       <c r="N66" t="s">
         <v>68</v>
       </c>
-      <c r="R66" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -4915,11 +4515,11 @@
       <c r="F67" t="s">
         <v>157</v>
       </c>
-      <c r="R67" t="s">
+      <c r="N67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>301</v>
       </c>
@@ -4932,11 +4532,11 @@
       <c r="F68" t="s">
         <v>157</v>
       </c>
-      <c r="R68" t="s">
+      <c r="N68" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -4949,11 +4549,11 @@
       <c r="F69" t="s">
         <v>143</v>
       </c>
-      <c r="R69" t="s">
+      <c r="N69" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>302</v>
       </c>
@@ -4966,11 +4566,11 @@
       <c r="F70" t="s">
         <v>309</v>
       </c>
-      <c r="R70" t="s">
+      <c r="N70" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>25</v>
       </c>
@@ -4983,14 +4583,14 @@
       <c r="F71" t="s">
         <v>144</v>
       </c>
-      <c r="P71" t="s">
+      <c r="L71" t="s">
         <v>194</v>
       </c>
-      <c r="R71" t="s">
+      <c r="N71" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>303</v>
       </c>
@@ -5003,14 +4603,14 @@
       <c r="F72" t="s">
         <v>310</v>
       </c>
-      <c r="P72" t="s">
+      <c r="L72" t="s">
         <v>308</v>
       </c>
-      <c r="R72" t="s">
+      <c r="N72" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -5023,11 +4623,11 @@
       <c r="F73" t="s">
         <v>145</v>
       </c>
-      <c r="R73" t="s">
+      <c r="N73" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>304</v>
       </c>
@@ -5040,11 +4640,11 @@
       <c r="F74" t="s">
         <v>311</v>
       </c>
-      <c r="R74" t="s">
+      <c r="N74" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -5057,27 +4657,27 @@
       <c r="F75" t="s">
         <v>159</v>
       </c>
-      <c r="R75" t="s">
+      <c r="N75" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B76" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B77" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>203</v>
       </c>
@@ -5085,7 +4685,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>35</v>
       </c>
@@ -5095,11 +4695,11 @@
       <c r="F79" t="s">
         <v>37</v>
       </c>
-      <c r="R79" t="s">
+      <c r="N79" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>325</v>
       </c>
@@ -5109,11 +4709,11 @@
       <c r="F80" t="s">
         <v>326</v>
       </c>
-      <c r="R80" t="s">
+      <c r="N80" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>27</v>
       </c>
@@ -5123,11 +4723,11 @@
       <c r="F81" t="s">
         <v>37</v>
       </c>
-      <c r="R81" t="s">
+      <c r="N81" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>318</v>
       </c>
@@ -5137,11 +4737,11 @@
       <c r="F82" t="s">
         <v>326</v>
       </c>
-      <c r="R82" t="s">
+      <c r="N82" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -5151,11 +4751,11 @@
       <c r="D83" t="s">
         <v>92</v>
       </c>
-      <c r="R83" t="s">
+      <c r="N83" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>319</v>
       </c>
@@ -5165,11 +4765,11 @@
       <c r="D84" t="s">
         <v>332</v>
       </c>
-      <c r="R84" t="s">
+      <c r="N84" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -5182,11 +4782,11 @@
       <c r="F85" t="s">
         <v>158</v>
       </c>
-      <c r="R85" t="s">
+      <c r="N85" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>320</v>
       </c>
@@ -5199,11 +4799,11 @@
       <c r="F86" t="s">
         <v>158</v>
       </c>
-      <c r="R86" t="s">
+      <c r="N86" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -5216,11 +4816,11 @@
       <c r="F87" t="s">
         <v>161</v>
       </c>
-      <c r="R87" t="s">
+      <c r="N87" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>321</v>
       </c>
@@ -5233,11 +4833,11 @@
       <c r="F88" t="s">
         <v>161</v>
       </c>
-      <c r="R88" t="s">
+      <c r="N88" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -5247,14 +4847,14 @@
       <c r="D89" t="s">
         <v>123</v>
       </c>
-      <c r="P89" t="s">
+      <c r="L89" t="s">
         <v>195</v>
       </c>
-      <c r="R89" t="s">
+      <c r="N89" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>322</v>
       </c>
@@ -5264,14 +4864,14 @@
       <c r="D90" t="s">
         <v>335</v>
       </c>
-      <c r="P90" t="s">
+      <c r="L90" t="s">
         <v>338</v>
       </c>
-      <c r="R90" t="s">
+      <c r="N90" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>29</v>
       </c>
@@ -5284,11 +4884,11 @@
       <c r="F91" t="s">
         <v>164</v>
       </c>
-      <c r="R91" t="s">
+      <c r="N91" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>323</v>
       </c>
@@ -5301,11 +4901,11 @@
       <c r="F92" t="s">
         <v>164</v>
       </c>
-      <c r="R92" t="s">
+      <c r="N92" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -5319,7 +4919,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>324</v>
       </c>
@@ -5333,12 +4933,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>189</v>
       </c>
@@ -5423,47 +5023,47 @@
         <v>184</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>26</v>
       </c>
@@ -5479,17 +5079,11 @@
       <c r="J121" t="s">
         <v>36</v>
       </c>
-      <c r="L121" t="s">
-        <v>36</v>
-      </c>
-      <c r="N121" t="s">
-        <v>36</v>
-      </c>
-      <c r="T121">
+      <c r="P121">
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>339</v>
       </c>
@@ -5505,13 +5099,7 @@
       <c r="J122" t="s">
         <v>340</v>
       </c>
-      <c r="L122" t="s">
-        <v>340</v>
-      </c>
-      <c r="N122" t="s">
-        <v>340</v>
-      </c>
-      <c r="T122">
+      <c r="P122">
         <v>100</v>
       </c>
     </row>
@@ -5530,13 +5118,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T122"/>
+  <dimension ref="A1:P122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N120" sqref="N120:N121"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5549,17 +5137,15 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
@@ -5588,40 +5174,28 @@
         <v>166</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>353</v>
+        <v>192</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>354</v>
+        <v>193</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>355</v>
+        <v>200</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>356</v>
+        <v>199</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="T1" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -5634,11 +5208,11 @@
       <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="R2" t="s">
+      <c r="N2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -5651,11 +5225,11 @@
       <c r="F3" t="s">
         <v>238</v>
       </c>
-      <c r="R3" t="s">
+      <c r="N3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -5669,16 +5243,10 @@
         <v>167</v>
       </c>
       <c r="J4" t="s">
-        <v>167</v>
-      </c>
-      <c r="L4" t="s">
-        <v>357</v>
-      </c>
-      <c r="N4" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -5692,16 +5260,10 @@
         <v>255</v>
       </c>
       <c r="J5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L5" t="s">
-        <v>358</v>
-      </c>
-      <c r="N5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -5715,16 +5277,10 @@
         <v>168</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
-      </c>
-      <c r="L6" t="s">
-        <v>359</v>
-      </c>
-      <c r="N6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
@@ -5738,16 +5294,10 @@
         <v>256</v>
       </c>
       <c r="J7" t="s">
-        <v>256</v>
-      </c>
-      <c r="L7" t="s">
-        <v>360</v>
-      </c>
-      <c r="N7" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -5761,16 +5311,10 @@
         <v>169</v>
       </c>
       <c r="J8" t="s">
-        <v>169</v>
-      </c>
-      <c r="L8" t="s">
-        <v>361</v>
-      </c>
-      <c r="N8" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -5784,16 +5328,10 @@
         <v>257</v>
       </c>
       <c r="J9" t="s">
-        <v>257</v>
-      </c>
-      <c r="L9" t="s">
-        <v>362</v>
-      </c>
-      <c r="N9" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -5807,16 +5345,10 @@
         <v>170</v>
       </c>
       <c r="J10" t="s">
-        <v>170</v>
-      </c>
-      <c r="L10" t="s">
-        <v>363</v>
-      </c>
-      <c r="N10" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -5830,16 +5362,10 @@
         <v>258</v>
       </c>
       <c r="J11" t="s">
-        <v>258</v>
-      </c>
-      <c r="L11" t="s">
-        <v>364</v>
-      </c>
-      <c r="N11" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -5853,16 +5379,10 @@
         <v>171</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
-      </c>
-      <c r="L12" t="s">
-        <v>365</v>
-      </c>
-      <c r="N12" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>244</v>
       </c>
@@ -5876,16 +5396,10 @@
         <v>259</v>
       </c>
       <c r="J13" t="s">
-        <v>259</v>
-      </c>
-      <c r="L13" t="s">
-        <v>366</v>
-      </c>
-      <c r="N13" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -5893,7 +5407,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -5904,7 +5418,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>260</v>
       </c>
@@ -6103,7 +5617,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -6114,7 +5628,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>264</v>
       </c>
@@ -6125,7 +5639,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -6136,7 +5650,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>265</v>
       </c>
@@ -6147,7 +5661,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -6158,7 +5672,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>130</v>
       </c>
@@ -6169,7 +5683,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>209</v>
       </c>
@@ -6180,7 +5694,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>346</v>
       </c>
@@ -6191,7 +5705,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -6202,7 +5716,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -6213,7 +5727,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>341</v>
       </c>
@@ -6224,7 +5738,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>344</v>
       </c>
@@ -6235,7 +5749,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -6246,7 +5760,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>266</v>
       </c>
@@ -6257,7 +5771,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -6274,19 +5788,13 @@
         <v>173</v>
       </c>
       <c r="J47" t="s">
-        <v>173</v>
-      </c>
-      <c r="L47" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="N47" t="s">
-        <v>367</v>
-      </c>
-      <c r="R47" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>267</v>
       </c>
@@ -6303,19 +5811,13 @@
         <v>282</v>
       </c>
       <c r="J48" t="s">
-        <v>282</v>
-      </c>
-      <c r="L48" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="N48" t="s">
-        <v>368</v>
-      </c>
-      <c r="R48" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -6332,19 +5834,13 @@
         <v>174</v>
       </c>
       <c r="J49" t="s">
-        <v>174</v>
-      </c>
-      <c r="L49" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="N49" t="s">
-        <v>369</v>
-      </c>
-      <c r="R49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>268</v>
       </c>
@@ -6361,19 +5857,13 @@
         <v>286</v>
       </c>
       <c r="J50" t="s">
-        <v>286</v>
-      </c>
-      <c r="L50" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="N50" t="s">
-        <v>370</v>
-      </c>
-      <c r="R50" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -6390,22 +5880,16 @@
         <v>175</v>
       </c>
       <c r="J51" t="s">
-        <v>175</v>
+        <v>367</v>
       </c>
       <c r="L51" t="s">
-        <v>371</v>
+        <v>191</v>
       </c>
       <c r="N51" t="s">
-        <v>371</v>
-      </c>
-      <c r="P51" t="s">
-        <v>191</v>
-      </c>
-      <c r="R51" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>269</v>
       </c>
@@ -6422,22 +5906,16 @@
         <v>290</v>
       </c>
       <c r="J52" t="s">
-        <v>290</v>
+        <v>368</v>
       </c>
       <c r="L52" t="s">
-        <v>372</v>
+        <v>298</v>
       </c>
       <c r="N52" t="s">
-        <v>372</v>
-      </c>
-      <c r="P52" t="s">
-        <v>298</v>
-      </c>
-      <c r="R52" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -6454,19 +5932,13 @@
         <v>176</v>
       </c>
       <c r="J53" t="s">
-        <v>176</v>
-      </c>
-      <c r="L53" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="N53" t="s">
-        <v>373</v>
-      </c>
-      <c r="R53" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>270</v>
       </c>
@@ -6483,19 +5955,13 @@
         <v>291</v>
       </c>
       <c r="J54" t="s">
-        <v>291</v>
-      </c>
-      <c r="L54" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="N54" t="s">
-        <v>374</v>
-      </c>
-      <c r="R54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -6509,19 +5975,13 @@
         <v>172</v>
       </c>
       <c r="J55" t="s">
-        <v>172</v>
-      </c>
-      <c r="L55" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="N55" t="s">
-        <v>375</v>
-      </c>
-      <c r="R55" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>271</v>
       </c>
@@ -6535,19 +5995,13 @@
         <v>289</v>
       </c>
       <c r="J56" t="s">
-        <v>289</v>
-      </c>
-      <c r="L56" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N56" t="s">
-        <v>376</v>
-      </c>
-      <c r="R56" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -6560,11 +6014,11 @@
       <c r="F57" t="s">
         <v>68</v>
       </c>
-      <c r="R57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
@@ -6572,7 +6026,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>205</v>
       </c>
@@ -6580,7 +6034,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>207</v>
       </c>
@@ -6593,11 +6047,11 @@
       <c r="F60" t="s">
         <v>208</v>
       </c>
-      <c r="R60" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -6616,17 +6070,11 @@
       <c r="J61" t="s">
         <v>68</v>
       </c>
-      <c r="L61" t="s">
-        <v>68</v>
-      </c>
       <c r="N61" t="s">
         <v>68</v>
       </c>
-      <c r="R61" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>299</v>
       </c>
@@ -6645,17 +6093,11 @@
       <c r="J62" t="s">
         <v>68</v>
       </c>
-      <c r="L62" t="s">
-        <v>68</v>
-      </c>
       <c r="N62" t="s">
         <v>68</v>
       </c>
-      <c r="R62" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -6674,17 +6116,11 @@
       <c r="J63" t="s">
         <v>68</v>
       </c>
-      <c r="L63" t="s">
-        <v>68</v>
-      </c>
       <c r="N63" t="s">
         <v>68</v>
       </c>
-      <c r="R63" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>300</v>
       </c>
@@ -6703,17 +6139,11 @@
       <c r="J64" t="s">
         <v>68</v>
       </c>
-      <c r="L64" t="s">
-        <v>68</v>
-      </c>
       <c r="N64" t="s">
         <v>68</v>
       </c>
-      <c r="R64" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -6726,11 +6156,11 @@
       <c r="F65" t="s">
         <v>157</v>
       </c>
-      <c r="R65" t="s">
+      <c r="N65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>301</v>
       </c>
@@ -6743,11 +6173,11 @@
       <c r="F66" t="s">
         <v>157</v>
       </c>
-      <c r="R66" t="s">
+      <c r="N66" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -6760,11 +6190,11 @@
       <c r="F67" t="s">
         <v>143</v>
       </c>
-      <c r="R67" t="s">
+      <c r="N67" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>302</v>
       </c>
@@ -6777,11 +6207,11 @@
       <c r="F68" t="s">
         <v>309</v>
       </c>
-      <c r="R68" t="s">
+      <c r="N68" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>25</v>
       </c>
@@ -6794,14 +6224,14 @@
       <c r="F69" t="s">
         <v>144</v>
       </c>
-      <c r="P69" t="s">
+      <c r="L69" t="s">
         <v>194</v>
       </c>
-      <c r="R69" t="s">
+      <c r="N69" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>303</v>
       </c>
@@ -6814,14 +6244,14 @@
       <c r="F70" t="s">
         <v>310</v>
       </c>
-      <c r="P70" t="s">
+      <c r="L70" t="s">
         <v>308</v>
       </c>
-      <c r="R70" t="s">
+      <c r="N70" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -6834,11 +6264,11 @@
       <c r="F71" t="s">
         <v>145</v>
       </c>
-      <c r="R71" t="s">
+      <c r="N71" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>304</v>
       </c>
@@ -6851,11 +6281,11 @@
       <c r="F72" t="s">
         <v>311</v>
       </c>
-      <c r="R72" t="s">
+      <c r="N72" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -6868,11 +6298,11 @@
       <c r="F73" t="s">
         <v>159</v>
       </c>
-      <c r="R73" t="s">
+      <c r="N73" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>133</v>
       </c>
@@ -6883,7 +6313,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>201</v>
       </c>
@@ -6894,7 +6324,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>203</v>
       </c>
@@ -6905,7 +6335,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>35</v>
       </c>
@@ -6915,11 +6345,11 @@
       <c r="F77" t="s">
         <v>37</v>
       </c>
-      <c r="R77" t="s">
+      <c r="N77" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>325</v>
       </c>
@@ -6929,11 +6359,11 @@
       <c r="F78" t="s">
         <v>326</v>
       </c>
-      <c r="R78" t="s">
+      <c r="N78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>27</v>
       </c>
@@ -6943,11 +6373,11 @@
       <c r="F79" t="s">
         <v>37</v>
       </c>
-      <c r="R79" t="s">
+      <c r="N79" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>318</v>
       </c>
@@ -6957,11 +6387,11 @@
       <c r="F80" t="s">
         <v>326</v>
       </c>
-      <c r="R80" t="s">
+      <c r="N80" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -6971,11 +6401,11 @@
       <c r="D81" t="s">
         <v>92</v>
       </c>
-      <c r="R81" t="s">
+      <c r="N81" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>319</v>
       </c>
@@ -6985,11 +6415,11 @@
       <c r="D82" t="s">
         <v>332</v>
       </c>
-      <c r="R82" t="s">
+      <c r="N82" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -7002,11 +6432,11 @@
       <c r="F83" t="s">
         <v>158</v>
       </c>
-      <c r="R83" t="s">
+      <c r="N83" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>320</v>
       </c>
@@ -7019,11 +6449,11 @@
       <c r="F84" t="s">
         <v>158</v>
       </c>
-      <c r="R84" t="s">
+      <c r="N84" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -7036,11 +6466,11 @@
       <c r="F85" t="s">
         <v>161</v>
       </c>
-      <c r="R85" t="s">
+      <c r="N85" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>321</v>
       </c>
@@ -7053,11 +6483,11 @@
       <c r="F86" t="s">
         <v>161</v>
       </c>
-      <c r="R86" t="s">
+      <c r="N86" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>28</v>
       </c>
@@ -7067,14 +6497,14 @@
       <c r="D87" t="s">
         <v>105</v>
       </c>
-      <c r="P87" t="s">
+      <c r="L87" t="s">
         <v>195</v>
       </c>
-      <c r="R87" t="s">
+      <c r="N87" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>322</v>
       </c>
@@ -7084,14 +6514,14 @@
       <c r="D88" t="s">
         <v>314</v>
       </c>
-      <c r="P88" t="s">
+      <c r="L88" t="s">
         <v>338</v>
       </c>
-      <c r="R88" t="s">
+      <c r="N88" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>29</v>
       </c>
@@ -7104,11 +6534,11 @@
       <c r="F89" t="s">
         <v>164</v>
       </c>
-      <c r="R89" t="s">
+      <c r="N89" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>323</v>
       </c>
@@ -7116,16 +6546,16 @@
         <v>307</v>
       </c>
       <c r="D90" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="F90" t="s">
         <v>164</v>
       </c>
-      <c r="R90" t="s">
+      <c r="N90" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>30</v>
       </c>
@@ -7139,7 +6569,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>324</v>
       </c>
@@ -7153,22 +6583,22 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>177</v>
       </c>
@@ -7253,37 +6683,37 @@
         <v>185</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>26</v>
       </c>
@@ -7299,19 +6729,13 @@
       <c r="J119" t="s">
         <v>36</v>
       </c>
-      <c r="L119" t="s">
-        <v>36</v>
-      </c>
-      <c r="N119" t="s">
-        <v>36</v>
-      </c>
-      <c r="T119">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P119">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B120" t="s">
         <v>340</v>
@@ -7325,16 +6749,13 @@
       <c r="J120" t="s">
         <v>340</v>
       </c>
-      <c r="L120" t="s">
-        <v>340</v>
-      </c>
-      <c r="N120" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P120">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B121" t="s">
         <v>340</v>
@@ -7348,14 +6769,11 @@
       <c r="J121" t="s">
         <v>340</v>
       </c>
-      <c r="L121" t="s">
-        <v>340</v>
-      </c>
-      <c r="N121" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P121">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>339</v>
       </c>
@@ -7371,14 +6789,8 @@
       <c r="J122" t="s">
         <v>340</v>
       </c>
-      <c r="L122" t="s">
-        <v>340</v>
-      </c>
-      <c r="N122" t="s">
-        <v>340</v>
-      </c>
-      <c r="T122">
-        <v>100</v>
+      <c r="P122">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -7398,14 +6810,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7427,6 +6839,9 @@
       <c r="B2" s="4" t="s">
         <v>148</v>
       </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -7443,9 +6858,6 @@
       <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4">
-        <v>60</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -7470,35 +6882,29 @@
       <c r="B7" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C7">
-        <v>60</v>
-      </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="C10">
-        <v>60</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -7511,10 +6917,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7525,7 +6931,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B1" t="s">
         <v>135</v>
@@ -7533,7 +6939,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B2" t="s">
         <v>151</v>
@@ -7541,10 +6947,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change modifiers to use short hand to allow them to work with other shift
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="519">
   <si>
     <t>a</t>
   </si>
@@ -1579,18 +1579,6 @@
     <t>Key Up</t>
   </si>
   <si>
-    <t>{Ctrl Down}</t>
-  </si>
-  <si>
-    <t>{Ctrl Up}</t>
-  </si>
-  <si>
-    <t>{Alt Down}</t>
-  </si>
-  <si>
-    <t>{Alt Up}</t>
-  </si>
-  <si>
     <t>x
 c</t>
   </si>
@@ -1631,18 +1619,6 @@
   <si>
     <t>.
 /</t>
-  </si>
-  <si>
-    <t>{LWin Down}</t>
-  </si>
-  <si>
-    <t>{LWin Up}</t>
-  </si>
-  <si>
-    <t>{RWin Down}</t>
-  </si>
-  <si>
-    <t>{RWin Up}</t>
   </si>
 </sst>
 </file>
@@ -16933,7 +16909,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16963,104 +16939,86 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C2">
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>507</v>
-      </c>
-      <c r="E2" t="s">
-        <v>508</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C3">
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>509</v>
-      </c>
-      <c r="E3" t="s">
-        <v>510</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C4">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>523</v>
-      </c>
-      <c r="E4" t="s">
-        <v>524</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C5">
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>507</v>
-      </c>
-      <c r="E5" t="s">
-        <v>508</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C6">
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>509</v>
-      </c>
-      <c r="E6" t="s">
-        <v>510</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C7">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>525</v>
-      </c>
-      <c r="E7" t="s">
-        <v>526</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Ctrl-Alt modifier combo support
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="524">
   <si>
     <t>a</t>
   </si>
@@ -1619,6 +1619,25 @@
   <si>
     <t>.
 /</t>
+  </si>
+  <si>
+    <t>LControl-Alt</t>
+  </si>
+  <si>
+    <t>z
+x
+c</t>
+  </si>
+  <si>
+    <t>RControl-Alt</t>
+  </si>
+  <si>
+    <t>,
+.
+/</t>
+  </si>
+  <si>
+    <t>^!</t>
   </si>
 </sst>
 </file>
@@ -6454,8 +6473,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Modifiers" displayName="Modifiers" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Modifiers" displayName="Modifiers" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Modifier"/>
     <tableColumn id="2" name="Keys" dataDxfId="138"/>
@@ -16906,10 +16925,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17019,6 +17038,34 @@
       </c>
       <c r="D7" t="s">
         <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>519</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>521</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved support for Green layer and mod keys.
</commit_message>
<xml_diff>
--- a/TextBlade.xlsx
+++ b/TextBlade.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Keys.DVORAK" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="562">
   <si>
     <t>a</t>
   </si>
@@ -1638,6 +1638,122 @@
   </si>
   <si>
     <t>^!</t>
+  </si>
+  <si>
+    <t>Space
+d
+f</t>
+  </si>
+  <si>
+    <t>Green Edit</t>
+  </si>
+  <si>
+    <t>Green Edit Down</t>
+  </si>
+  <si>
+    <t>Green Edit Up</t>
+  </si>
+  <si>
+    <t>{PgUp}</t>
+  </si>
+  <si>
+    <t>{Blind}{PgUp}</t>
+  </si>
+  <si>
+    <t>{PgDn}</t>
+  </si>
+  <si>
+    <t>{Blind}{PgDn}</t>
+  </si>
+  <si>
+    <t>{Blind}^{Home}</t>
+  </si>
+  <si>
+    <t>{Blind}^{End}</t>
+  </si>
+  <si>
+    <t>*1</t>
+  </si>
+  <si>
+    <t>*2</t>
+  </si>
+  <si>
+    <t>*3</t>
+  </si>
+  <si>
+    <t>*4</t>
+  </si>
+  <si>
+    <t>*5</t>
+  </si>
+  <si>
+    <t>*6</t>
+  </si>
+  <si>
+    <t>*7</t>
+  </si>
+  <si>
+    <t>*8</t>
+  </si>
+  <si>
+    <t>*9</t>
+  </si>
+  <si>
+    <t>*0</t>
+  </si>
+  <si>
+    <t>*-</t>
+  </si>
+  <si>
+    <t>*=</t>
+  </si>
+  <si>
+    <t>CtrlGreen</t>
+  </si>
+  <si>
+    <t>^Space</t>
+  </si>
+  <si>
+    <t>CtrlShiftGreen</t>
+  </si>
+  <si>
+    <t>+^Space</t>
+  </si>
+  <si>
+    <t>+!Space</t>
+  </si>
+  <si>
+    <t>+#Space</t>
+  </si>
+  <si>
+    <t>+#^Space</t>
+  </si>
+  <si>
+    <t>+#!Space</t>
+  </si>
+  <si>
+    <t>+^!Space</t>
+  </si>
+  <si>
+    <t>+#!^Space</t>
+  </si>
+  <si>
+    <t>CtrlAltGreen</t>
+  </si>
+  <si>
+    <t>^!Space</t>
+  </si>
+  <si>
+    <t>AltShiftGreen</t>
+  </si>
+  <si>
+    <t>CtrlAltShiftGreen</t>
+  </si>
+  <si>
+    <t>AltGreen</t>
+  </si>
+  <si>
+    <t>!Space</t>
   </si>
 </sst>
 </file>
@@ -6423,9 +6539,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:P153" totalsRowShown="0" headerRowDxfId="140">
-  <autoFilter ref="A1:P153"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="HotKeys.QWERTY" displayName="HotKeys.QWERTY" ref="A1:R159" totalsRowShown="0" headerRowDxfId="140">
+  <autoFilter ref="A1:R159"/>
+  <tableColumns count="18">
     <tableColumn id="1" name="Hotkey"/>
     <tableColumn id="2" name="Alpha Down"/>
     <tableColumn id="3" name="Alpha Up"/>
@@ -6441,6 +6557,8 @@
     <tableColumn id="12" name="Media Up"/>
     <tableColumn id="10" name="Green Media Down"/>
     <tableColumn id="13" name="Green Media Up"/>
+    <tableColumn id="15" name="Green Edit Down"/>
+    <tableColumn id="16" name="Green Edit Up"/>
     <tableColumn id="14" name="Delay"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6487,8 +6605,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Layers" displayName="Layers" ref="A1:C17" totalsRowShown="0">
+  <autoFilter ref="A1:C17"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Layer"/>
     <tableColumn id="2" name="Keys" dataDxfId="137"/>
@@ -6499,8 +6617,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="LayerAliases" displayName="LayerAliases" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="LayerAliases" displayName="LayerAliases" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10"/>
   <tableColumns count="2">
     <tableColumn id="1" name="LayerAlias"/>
     <tableColumn id="2" name="Layer"/>
@@ -13191,13 +13309,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P153"/>
+  <dimension ref="A1:R159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D94" sqref="D94"/>
+      <selection pane="bottomRight" activeCell="A159" sqref="A159:XFD159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13215,10 +13333,11 @@
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
@@ -13265,10 +13384,16 @@
         <v>199</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -13284,8 +13409,11 @@
       <c r="N2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -13301,8 +13429,11 @@
       <c r="N3" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -13319,7 +13450,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -13336,7 +13467,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -13353,7 +13484,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
@@ -13370,7 +13501,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -13387,7 +13518,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -13404,7 +13535,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -13421,7 +13552,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -13438,7 +13569,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -13455,7 +13586,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>244</v>
       </c>
@@ -13472,7 +13603,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -13480,7 +13611,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>482</v>
       </c>
@@ -13488,7 +13619,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -13499,7 +13630,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>466</v>
       </c>
@@ -13507,7 +13638,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>467</v>
       </c>
@@ -13515,7 +13646,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>260</v>
       </c>
@@ -13526,7 +13657,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -13542,8 +13673,14 @@
       <c r="G20" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>126</v>
       </c>
@@ -13554,7 +13691,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>213</v>
       </c>
@@ -13565,7 +13702,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>216</v>
       </c>
@@ -13581,8 +13718,14 @@
       <c r="G23" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -13593,7 +13736,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>129</v>
       </c>
@@ -13604,7 +13747,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>223</v>
       </c>
@@ -13615,7 +13758,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>224</v>
       </c>
@@ -13626,7 +13769,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>225</v>
       </c>
@@ -13637,7 +13780,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>226</v>
       </c>
@@ -13648,7 +13791,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>233</v>
       </c>
@@ -13659,7 +13802,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>227</v>
       </c>
@@ -13670,7 +13813,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>235</v>
       </c>
@@ -13839,7 +13982,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>346</v>
       </c>
@@ -13850,7 +13993,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -13861,7 +14004,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>94</v>
       </c>
@@ -13872,7 +14015,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>341</v>
       </c>
@@ -13883,7 +14026,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>344</v>
       </c>
@@ -13894,7 +14037,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -13905,7 +14048,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>487</v>
       </c>
@@ -13913,7 +14056,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>488</v>
       </c>
@@ -13921,7 +14064,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>266</v>
       </c>
@@ -13932,7 +14075,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -13954,8 +14097,11 @@
       <c r="N58" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>267</v>
       </c>
@@ -13977,8 +14123,11 @@
       <c r="N59" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P59" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -14000,8 +14149,11 @@
       <c r="N60" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>268</v>
       </c>
@@ -14023,8 +14175,11 @@
       <c r="N61" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P61" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -14049,8 +14204,11 @@
       <c r="N62" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P62" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>269</v>
       </c>
@@ -14075,8 +14233,11 @@
       <c r="N63" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -14098,8 +14259,11 @@
       <c r="N64" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>270</v>
       </c>
@@ -14121,8 +14285,11 @@
       <c r="N65" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -14142,7 +14309,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>271</v>
       </c>
@@ -14162,7 +14329,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>31</v>
       </c>
@@ -14178,8 +14345,11 @@
       <c r="N68" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
@@ -14187,7 +14357,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>205</v>
       </c>
@@ -14195,7 +14365,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>207</v>
       </c>
@@ -14211,8 +14381,11 @@
       <c r="N71" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P71" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>32</v>
       </c>
@@ -14234,8 +14407,11 @@
       <c r="N72" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>299</v>
       </c>
@@ -14257,8 +14433,11 @@
       <c r="N73" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>33</v>
       </c>
@@ -14280,8 +14459,11 @@
       <c r="N74" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>300</v>
       </c>
@@ -14303,8 +14485,11 @@
       <c r="N75" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P75" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -14320,8 +14505,11 @@
       <c r="N76" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P76" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>500</v>
       </c>
@@ -14334,8 +14522,11 @@
       <c r="N77" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>501</v>
       </c>
@@ -14348,8 +14539,11 @@
       <c r="N78" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P78" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>301</v>
       </c>
@@ -14365,8 +14559,11 @@
       <c r="N79" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -14382,8 +14579,11 @@
       <c r="N80" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P80" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>502</v>
       </c>
@@ -14396,8 +14596,11 @@
       <c r="N81" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P81" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>503</v>
       </c>
@@ -14410,8 +14613,11 @@
       <c r="N82" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P82" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>302</v>
       </c>
@@ -14427,8 +14633,11 @@
       <c r="N83" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P83" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>25</v>
       </c>
@@ -14447,8 +14656,11 @@
       <c r="N84" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P84" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>471</v>
       </c>
@@ -14464,8 +14676,11 @@
       <c r="N85" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P85" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>472</v>
       </c>
@@ -14481,8 +14696,11 @@
       <c r="N86" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P86" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>303</v>
       </c>
@@ -14501,8 +14719,11 @@
       <c r="N87" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P87" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -14518,8 +14739,11 @@
       <c r="N88" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P88" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>469</v>
       </c>
@@ -14532,8 +14756,11 @@
       <c r="N89" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P89" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>470</v>
       </c>
@@ -14546,8 +14773,11 @@
       <c r="N90" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P90" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>304</v>
       </c>
@@ -14563,8 +14793,11 @@
       <c r="N91" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P91" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>34</v>
       </c>
@@ -14580,8 +14813,11 @@
       <c r="N92" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P92" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>133</v>
       </c>
@@ -14589,7 +14825,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>201</v>
       </c>
@@ -14597,7 +14833,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>203</v>
       </c>
@@ -14608,19 +14844,19 @@
         <v>479</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>325</v>
       </c>
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>27</v>
       </c>
@@ -14633,8 +14869,11 @@
       <c r="N98" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P98" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>318</v>
       </c>
@@ -14647,8 +14886,11 @@
       <c r="N99" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P99" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -14662,7 +14904,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>486</v>
       </c>
@@ -14670,7 +14912,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>485</v>
       </c>
@@ -14678,7 +14920,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>319</v>
       </c>
@@ -14692,7 +14934,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>12</v>
       </c>
@@ -14708,8 +14950,11 @@
       <c r="N104" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P104" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>491</v>
       </c>
@@ -14722,8 +14967,11 @@
       <c r="N105" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P105" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>492</v>
       </c>
@@ -14736,8 +14984,11 @@
       <c r="N106" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P106" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>320</v>
       </c>
@@ -14753,8 +15004,11 @@
       <c r="N107" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P107" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -14770,8 +15024,11 @@
       <c r="N108" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P108" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>489</v>
       </c>
@@ -14784,8 +15041,11 @@
       <c r="N109" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P109" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>490</v>
       </c>
@@ -14798,8 +15058,11 @@
       <c r="N110" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P110" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>321</v>
       </c>
@@ -14815,8 +15078,11 @@
       <c r="N111" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P111" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>28</v>
       </c>
@@ -14833,7 +15099,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>484</v>
       </c>
@@ -14847,7 +15113,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>493</v>
       </c>
@@ -14862,7 +15128,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>322</v>
       </c>
@@ -14879,7 +15145,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>29</v>
       </c>
@@ -14895,8 +15161,11 @@
       <c r="N116" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P116" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>494</v>
       </c>
@@ -14909,8 +15178,11 @@
       <c r="N117" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P117" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>495</v>
       </c>
@@ -14923,8 +15195,11 @@
       <c r="N118" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P118" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>323</v>
       </c>
@@ -14940,8 +15215,11 @@
       <c r="N119" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P119" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>30</v>
       </c>
@@ -14954,8 +15232,11 @@
       <c r="F120" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P120" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>473</v>
       </c>
@@ -14965,8 +15246,11 @@
       <c r="F121" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P121" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>474</v>
       </c>
@@ -14976,8 +15260,11 @@
       <c r="F122" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P122" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>324</v>
       </c>
@@ -14990,138 +15277,213 @@
       <c r="F123" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P123" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+        <v>534</v>
+      </c>
+      <c r="B127" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+      <c r="B129" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+      <c r="B131" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+      <c r="B133" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+      <c r="B135" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+      <c r="B137" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+      <c r="B139" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+      <c r="B141" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+      <c r="B143" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="B145" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+      <c r="B147" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+      <c r="B149" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>26</v>
       </c>
@@ -15137,11 +15499,11 @@
       <c r="J150" t="s">
         <v>36</v>
       </c>
-      <c r="P150">
+      <c r="R150">
         <v>130</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>390</v>
       </c>
@@ -15157,13 +15519,13 @@
       <c r="J151" t="s">
         <v>340</v>
       </c>
-      <c r="P151">
+      <c r="R151">
         <v>130</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>391</v>
+        <v>549</v>
       </c>
       <c r="B152" t="s">
         <v>340</v>
@@ -15177,13 +15539,13 @@
       <c r="J152" t="s">
         <v>340</v>
       </c>
-      <c r="P152">
+      <c r="R152">
         <v>130</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>339</v>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>550</v>
       </c>
       <c r="B153" t="s">
         <v>340</v>
@@ -15197,7 +15559,127 @@
       <c r="J153" t="s">
         <v>340</v>
       </c>
-      <c r="P153">
+      <c r="R153">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B154" t="s">
+        <v>340</v>
+      </c>
+      <c r="F154" t="s">
+        <v>340</v>
+      </c>
+      <c r="H154" t="s">
+        <v>340</v>
+      </c>
+      <c r="J154" t="s">
+        <v>340</v>
+      </c>
+      <c r="R154">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B155" t="s">
+        <v>340</v>
+      </c>
+      <c r="F155" t="s">
+        <v>340</v>
+      </c>
+      <c r="H155" t="s">
+        <v>340</v>
+      </c>
+      <c r="J155" t="s">
+        <v>340</v>
+      </c>
+      <c r="R155">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B156" t="s">
+        <v>340</v>
+      </c>
+      <c r="F156" t="s">
+        <v>340</v>
+      </c>
+      <c r="H156" t="s">
+        <v>340</v>
+      </c>
+      <c r="J156" t="s">
+        <v>340</v>
+      </c>
+      <c r="R156">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B157" t="s">
+        <v>340</v>
+      </c>
+      <c r="F157" t="s">
+        <v>340</v>
+      </c>
+      <c r="H157" t="s">
+        <v>340</v>
+      </c>
+      <c r="J157" t="s">
+        <v>340</v>
+      </c>
+      <c r="R157">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B158" t="s">
+        <v>340</v>
+      </c>
+      <c r="F158" t="s">
+        <v>340</v>
+      </c>
+      <c r="H158" t="s">
+        <v>340</v>
+      </c>
+      <c r="J158" t="s">
+        <v>340</v>
+      </c>
+      <c r="R158">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>339</v>
+      </c>
+      <c r="B159" t="s">
+        <v>340</v>
+      </c>
+      <c r="F159" t="s">
+        <v>340</v>
+      </c>
+      <c r="H159" t="s">
+        <v>340</v>
+      </c>
+      <c r="J159" t="s">
+        <v>340</v>
+      </c>
+      <c r="R159">
         <v>130</v>
       </c>
     </row>
@@ -16927,7 +17409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -17079,16 +17561,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17140,6 +17622,9 @@
       <c r="B5" s="4" t="s">
         <v>196</v>
       </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -17148,6 +17633,9 @@
       <c r="B6" s="4" t="s">
         <v>155</v>
       </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -17164,6 +17652,9 @@
       <c r="B8" s="4" t="s">
         <v>348</v>
       </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -17172,6 +17663,9 @@
       <c r="B9" s="4" t="s">
         <v>349</v>
       </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -17179,6 +17673,86 @@
       </c>
       <c r="B10" s="5" t="s">
         <v>390</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>525</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>546</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>548</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>556</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>558</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>559</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>560</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -17192,10 +17766,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17234,6 +17808,54 @@
       </c>
       <c r="B4" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>546</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>558</v>
+      </c>
+      <c r="B8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>559</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>560</v>
+      </c>
+      <c r="B10" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>